<commit_message>
Add: Actual lineup for 2_1, with updated lua script to extract data from wt;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15649" uniqueCount="5223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15645" uniqueCount="5223">
   <si>
     <t>Vehicles</t>
   </si>
@@ -2240,6 +2240,30 @@
     <t>КВ-1 (Л-11)</t>
   </si>
   <si>
+    <t>ussr_t_34_1941</t>
+  </si>
+  <si>
+    <t>T-34 (1941)</t>
+  </si>
+  <si>
+    <t>Т-34 (1941)</t>
+  </si>
+  <si>
+    <t>ussr_t_34_1941_cast_turret</t>
+  </si>
+  <si>
+    <t>T-34 (1st Gv.T.Br.)</t>
+  </si>
+  <si>
+    <t>Т-34 (1 Гв.Т.Бр.)</t>
+  </si>
+  <si>
+    <t>T-34 1941 (1st Gv.T.Br.)</t>
+  </si>
+  <si>
+    <t>Т-34 1941 (1 Гв.Т.Бр.)</t>
+  </si>
+  <si>
     <t>ussr_smk</t>
   </si>
   <si>
@@ -2256,30 +2280,6 @@
   </si>
   <si>
     <t>Т-34Э</t>
-  </si>
-  <si>
-    <t>ussr_t_34_1941</t>
-  </si>
-  <si>
-    <t>T-34 (1941)</t>
-  </si>
-  <si>
-    <t>Т-34 (1941)</t>
-  </si>
-  <si>
-    <t>ussr_t_34_1941_cast_turret</t>
-  </si>
-  <si>
-    <t>T-34 (1st Gv.T.Br.)</t>
-  </si>
-  <si>
-    <t>Т-34 (1 Гв.Т.Бр.)</t>
-  </si>
-  <si>
-    <t>T-34 1941 (1st Gv.T.Br.)</t>
-  </si>
-  <si>
-    <t>Т-34 1941 (1 Гв.Т.Бр.)</t>
   </si>
   <si>
     <t>ussr_t_34E_STZ</t>
@@ -22989,9 +22989,6 @@
       <c r="J236" t="s">
         <v>27</v>
       </c>
-      <c r="K236" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
@@ -23013,21 +23010,18 @@
         <v>747</v>
       </c>
       <c r="G237" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="H237" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="J237" t="s">
         <v>27</v>
       </c>
-      <c r="K237" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B238" t="s">
         <v>22</v>
@@ -23039,24 +23033,24 @@
         <v>698</v>
       </c>
       <c r="E238" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="F238" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="G238" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="H238" t="s">
-        <v>750</v>
-      </c>
-      <c r="J238" t="s">
+        <v>752</v>
+      </c>
+      <c r="K238" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B239" t="s">
         <v>22</v>
@@ -23068,10 +23062,10 @@
         <v>698</v>
       </c>
       <c r="E239" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="F239" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="G239" t="s">
         <v>754</v>
@@ -23079,7 +23073,7 @@
       <c r="H239" t="s">
         <v>755</v>
       </c>
-      <c r="J239" t="s">
+      <c r="K239" t="s">
         <v>27</v>
       </c>
     </row>
@@ -23198,9 +23192,6 @@
       <c r="H243" t="s">
         <v>767</v>
       </c>
-      <c r="J243" t="s">
-        <v>27</v>
-      </c>
       <c r="K243" t="s">
         <v>27</v>
       </c>
@@ -23421,9 +23412,6 @@
       </c>
       <c r="H250" t="s">
         <v>787</v>
-      </c>
-      <c r="J250" t="s">
-        <v>27</v>
       </c>
       <c r="K250" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Add: Actual lineup for 5_1;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15645" uniqueCount="5223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15632" uniqueCount="5223">
   <si>
     <t>Vehicles</t>
   </si>
@@ -3839,6 +3839,15 @@
     <t>"Пантера"</t>
   </si>
   <si>
+    <t>sw_strv_74</t>
+  </si>
+  <si>
+    <t>Strv 74</t>
+  </si>
+  <si>
+    <t>Stridsvagn 74</t>
+  </si>
+  <si>
     <t>sw_ikv_103</t>
   </si>
   <si>
@@ -3846,15 +3855,6 @@
   </si>
   <si>
     <t>Infanterikanonvagn 103</t>
-  </si>
-  <si>
-    <t>sw_strv_74</t>
-  </si>
-  <si>
-    <t>Strv 74</t>
-  </si>
-  <si>
-    <t>Stridsvagn 74</t>
   </si>
   <si>
     <t>uk_a_43_black_prince</t>
@@ -21869,9 +21869,6 @@
       <c r="L201" t="s">
         <v>64</v>
       </c>
-      <c r="M201" t="s">
-        <v>64</v>
-      </c>
       <c r="N201" t="s">
         <v>64</v>
       </c>
@@ -22765,9 +22762,6 @@
       <c r="L229" t="s">
         <v>64</v>
       </c>
-      <c r="M229" t="s">
-        <v>64</v>
-      </c>
       <c r="N229" t="s">
         <v>64</v>
       </c>
@@ -25093,6 +25087,9 @@
       <c r="L304" t="s">
         <v>64</v>
       </c>
+      <c r="M304" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
@@ -25186,9 +25183,6 @@
       <c r="L307" t="s">
         <v>27</v>
       </c>
-      <c r="M307" t="s">
-        <v>27</v>
-      </c>
       <c r="N307" t="s">
         <v>27</v>
       </c>
@@ -25288,9 +25282,6 @@
       <c r="L310" t="s">
         <v>27</v>
       </c>
-      <c r="M310" t="s">
-        <v>27</v>
-      </c>
       <c r="N310" t="s">
         <v>27</v>
       </c>
@@ -26096,9 +26087,6 @@
       <c r="H336" t="s">
         <v>1047</v>
       </c>
-      <c r="M336" t="s">
-        <v>27</v>
-      </c>
       <c r="N336" t="s">
         <v>27</v>
       </c>
@@ -26881,6 +26869,9 @@
       <c r="L361" t="s">
         <v>64</v>
       </c>
+      <c r="M361" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="s">
@@ -27061,9 +27052,6 @@
       <c r="L367" t="s">
         <v>27</v>
       </c>
-      <c r="M367" t="s">
-        <v>27</v>
-      </c>
       <c r="N367" t="s">
         <v>27</v>
       </c>
@@ -27163,9 +27151,6 @@
       <c r="H370" t="s">
         <v>1141</v>
       </c>
-      <c r="M370" t="s">
-        <v>27</v>
-      </c>
       <c r="N370" t="s">
         <v>27</v>
       </c>
@@ -28657,9 +28642,6 @@
       <c r="N418" t="s">
         <v>27</v>
       </c>
-      <c r="O418" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
@@ -28686,11 +28668,11 @@
       <c r="H419" t="s">
         <v>1280</v>
       </c>
-      <c r="M419" t="s">
-        <v>27</v>
-      </c>
       <c r="N419" t="s">
         <v>27</v>
+      </c>
+      <c r="O419" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="420">
@@ -29976,9 +29958,6 @@
       <c r="H461" t="s">
         <v>1399</v>
       </c>
-      <c r="M461" t="s">
-        <v>27</v>
-      </c>
       <c r="N461" t="s">
         <v>27</v>
       </c>
@@ -30139,9 +30118,6 @@
       <c r="H466" t="s">
         <v>1412</v>
       </c>
-      <c r="M466" t="s">
-        <v>64</v>
-      </c>
       <c r="N466" t="s">
         <v>64</v>
       </c>
@@ -30174,9 +30150,6 @@
       <c r="H467" t="s">
         <v>1414</v>
       </c>
-      <c r="M467" t="s">
-        <v>64</v>
-      </c>
       <c r="N467" t="s">
         <v>64</v>
       </c>
@@ -30305,9 +30278,6 @@
       <c r="H471" t="s">
         <v>1427</v>
       </c>
-      <c r="M471" t="s">
-        <v>27</v>
-      </c>
       <c r="N471" t="s">
         <v>27</v>
       </c>
@@ -31618,9 +31588,6 @@
       <c r="H514" t="s">
         <v>1550</v>
       </c>
-      <c r="M514" t="s">
-        <v>64</v>
-      </c>
       <c r="N514" t="s">
         <v>64</v>
       </c>
@@ -31851,9 +31818,6 @@
       <c r="H521" t="s">
         <v>1570</v>
       </c>
-      <c r="M521" t="s">
-        <v>27</v>
-      </c>
       <c r="N521" t="s">
         <v>27</v>
       </c>
@@ -31885,9 +31849,6 @@
       </c>
       <c r="H522" t="s">
         <v>1573</v>
-      </c>
-      <c r="M522" t="s">
-        <v>27</v>
       </c>
       <c r="N522" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Add: Actual lineup for 4_1; Fix: LineupListViewModel is now singleton, and all events passed correctly to only one instance from a view;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15632" uniqueCount="5223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15643" uniqueCount="5223">
   <si>
     <t>Vehicles</t>
   </si>
@@ -21869,6 +21869,9 @@
       <c r="L201" t="s">
         <v>64</v>
       </c>
+      <c r="M201" t="s">
+        <v>64</v>
+      </c>
       <c r="N201" t="s">
         <v>64</v>
       </c>
@@ -22762,6 +22765,9 @@
       <c r="L229" t="s">
         <v>64</v>
       </c>
+      <c r="M229" t="s">
+        <v>64</v>
+      </c>
       <c r="N229" t="s">
         <v>64</v>
       </c>
@@ -25183,6 +25189,9 @@
       <c r="L307" t="s">
         <v>27</v>
       </c>
+      <c r="M307" t="s">
+        <v>27</v>
+      </c>
       <c r="N307" t="s">
         <v>27</v>
       </c>
@@ -25282,6 +25291,9 @@
       <c r="L310" t="s">
         <v>27</v>
       </c>
+      <c r="M310" t="s">
+        <v>27</v>
+      </c>
       <c r="N310" t="s">
         <v>27</v>
       </c>
@@ -28668,6 +28680,9 @@
       <c r="H419" t="s">
         <v>1280</v>
       </c>
+      <c r="M419" t="s">
+        <v>27</v>
+      </c>
       <c r="N419" t="s">
         <v>27</v>
       </c>
@@ -29958,6 +29973,9 @@
       <c r="H461" t="s">
         <v>1399</v>
       </c>
+      <c r="M461" t="s">
+        <v>27</v>
+      </c>
       <c r="N461" t="s">
         <v>27</v>
       </c>
@@ -30118,6 +30136,9 @@
       <c r="H466" t="s">
         <v>1412</v>
       </c>
+      <c r="M466" t="s">
+        <v>64</v>
+      </c>
       <c r="N466" t="s">
         <v>64</v>
       </c>
@@ -30150,6 +30171,9 @@
       <c r="H467" t="s">
         <v>1414</v>
       </c>
+      <c r="M467" t="s">
+        <v>64</v>
+      </c>
       <c r="N467" t="s">
         <v>64</v>
       </c>
@@ -30278,6 +30302,9 @@
       <c r="H471" t="s">
         <v>1427</v>
       </c>
+      <c r="M471" t="s">
+        <v>27</v>
+      </c>
       <c r="N471" t="s">
         <v>27</v>
       </c>
@@ -31588,6 +31615,9 @@
       <c r="H514" t="s">
         <v>1550</v>
       </c>
+      <c r="M514" t="s">
+        <v>64</v>
+      </c>
       <c r="N514" t="s">
         <v>64</v>
       </c>
@@ -31652,9 +31682,6 @@
       <c r="H516" t="s">
         <v>1556</v>
       </c>
-      <c r="M516" t="s">
-        <v>64</v>
-      </c>
       <c r="N516" t="s">
         <v>64</v>
       </c>
@@ -31818,6 +31845,9 @@
       <c r="H521" t="s">
         <v>1570</v>
       </c>
+      <c r="M521" t="s">
+        <v>27</v>
+      </c>
       <c r="N521" t="s">
         <v>27</v>
       </c>
@@ -31849,6 +31879,9 @@
       </c>
       <c r="H522" t="s">
         <v>1573</v>
+      </c>
+      <c r="M522" t="s">
+        <v>27</v>
       </c>
       <c r="N522" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Add: Data from LineupRequestInteractor now shows in a fragment, and updates it if necessary; Fix: View oversize on note 4;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15677" uniqueCount="5233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15676" uniqueCount="5233">
   <si>
     <t>Vehicles</t>
   </si>
@@ -32088,9 +32088,6 @@
       <c r="P527" t="s">
         <v>64</v>
       </c>
-      <c r="Q527" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="528">
       <c r="A528" t="s">

</xml_diff>

<commit_message>
Del: Old code that is not used any more;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11465" uniqueCount="3483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11466" uniqueCount="3483">
   <si>
     <t>Vehicles</t>
   </si>
@@ -8723,6 +8723,12 @@
     <t>Tank, Combat, Full Tracked, 105-mm Gun IPM1</t>
   </si>
   <si>
+    <t>us_m60a3_slep</t>
+  </si>
+  <si>
+    <t>M60 AMBT</t>
+  </si>
+  <si>
     <t>f-104g_china</t>
   </si>
   <si>
@@ -10437,12 +10443,6 @@
   </si>
   <si>
     <t>md_460_usa</t>
-  </si>
-  <si>
-    <t>us_m60a3_slep</t>
-  </si>
-  <si>
-    <t>M60 AMBT</t>
   </si>
   <si>
     <t>germ_leopard_2a5_yt_cup_2019</t>
@@ -43274,10 +43274,10 @@
         <v>2903</v>
       </c>
       <c r="B1474" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C1474" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D1474" t="s">
         <v>2873</v>
@@ -43286,7 +43286,7 @@
         <v>2904</v>
       </c>
       <c r="O1474" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1475">
@@ -43297,7 +43297,7 @@
         <v>113</v>
       </c>
       <c r="C1475" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D1475" t="s">
         <v>2873</v>
@@ -43306,7 +43306,7 @@
         <v>2906</v>
       </c>
       <c r="O1475" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1476">
@@ -43323,7 +43323,7 @@
         <v>2873</v>
       </c>
       <c r="E1476" t="s">
-        <v>2904</v>
+        <v>2908</v>
       </c>
       <c r="O1476" t="s">
         <v>48</v>
@@ -43331,19 +43331,19 @@
     </row>
     <row r="1477">
       <c r="A1477" t="s">
-        <v>2908</v>
+        <v>2909</v>
       </c>
       <c r="B1477" t="s">
         <v>113</v>
       </c>
       <c r="C1477" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1477" t="s">
         <v>2873</v>
       </c>
       <c r="E1477" t="s">
-        <v>2909</v>
+        <v>2906</v>
       </c>
       <c r="O1477" t="s">
         <v>48</v>
@@ -43357,7 +43357,7 @@
         <v>113</v>
       </c>
       <c r="C1478" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1478" t="s">
         <v>2873</v>
@@ -43394,10 +43394,10 @@
         <v>2914</v>
       </c>
       <c r="B1480" t="s">
-        <v>2519</v>
+        <v>113</v>
       </c>
       <c r="C1480" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D1480" t="s">
         <v>2873</v>
@@ -43406,9 +43406,6 @@
         <v>2915</v>
       </c>
       <c r="O1480" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1480" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43443,7 +43440,7 @@
         <v>2519</v>
       </c>
       <c r="C1482" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D1482" t="s">
         <v>2873</v>
@@ -43466,7 +43463,7 @@
         <v>2519</v>
       </c>
       <c r="C1483" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D1483" t="s">
         <v>2873</v>
@@ -43475,6 +43472,9 @@
         <v>2921</v>
       </c>
       <c r="O1483" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1483" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43486,7 +43486,7 @@
         <v>2519</v>
       </c>
       <c r="C1484" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1484" t="s">
         <v>2873</v>
@@ -43495,10 +43495,7 @@
         <v>2923</v>
       </c>
       <c r="O1484" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1484" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1485">
@@ -43532,7 +43529,7 @@
         <v>2519</v>
       </c>
       <c r="C1486" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1486" t="s">
         <v>2873</v>
@@ -43541,7 +43538,10 @@
         <v>2927</v>
       </c>
       <c r="O1486" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="P1486" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1487">
@@ -43552,7 +43552,7 @@
         <v>2519</v>
       </c>
       <c r="C1487" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1487" t="s">
         <v>2873</v>
@@ -43561,9 +43561,6 @@
         <v>2929</v>
       </c>
       <c r="O1487" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1487" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43586,6 +43583,9 @@
       <c r="O1488" t="s">
         <v>48</v>
       </c>
+      <c r="P1488" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="1489">
       <c r="A1489" t="s">
@@ -43632,41 +43632,41 @@
         <v>2936</v>
       </c>
       <c r="B1491" t="s">
-        <v>19</v>
+        <v>2519</v>
       </c>
       <c r="C1491" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="D1491" t="s">
+        <v>2873</v>
+      </c>
+      <c r="E1491" t="s">
         <v>2937</v>
       </c>
-      <c r="E1491" t="s">
-        <v>2938</v>
-      </c>
       <c r="O1491" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1491" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="1492">
       <c r="A1492" t="s">
+        <v>2938</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1492" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1492" t="s">
         <v>2939</v>
-      </c>
-      <c r="B1492" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1492" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1492" t="s">
-        <v>2937</v>
       </c>
       <c r="E1492" t="s">
         <v>2940</v>
       </c>
       <c r="O1492" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1492" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43678,19 +43678,16 @@
         <v>19</v>
       </c>
       <c r="C1493" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D1493" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1493" t="s">
         <v>2942</v>
       </c>
       <c r="O1493" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1493" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1494">
@@ -43704,7 +43701,7 @@
         <v>74</v>
       </c>
       <c r="D1494" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1494" t="s">
         <v>2944</v>
@@ -43724,16 +43721,19 @@
         <v>19</v>
       </c>
       <c r="C1495" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D1495" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1495" t="s">
         <v>2946</v>
       </c>
       <c r="O1495" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="P1495" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1496">
@@ -43747,7 +43747,7 @@
         <v>88</v>
       </c>
       <c r="D1496" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1496" t="s">
         <v>2948</v>
@@ -43764,18 +43764,15 @@
         <v>19</v>
       </c>
       <c r="C1497" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D1497" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1497" t="s">
         <v>2950</v>
       </c>
       <c r="O1497" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1497" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43790,12 +43787,15 @@
         <v>95</v>
       </c>
       <c r="D1498" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1498" t="s">
         <v>2952</v>
       </c>
       <c r="O1498" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1498" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43807,18 +43807,15 @@
         <v>19</v>
       </c>
       <c r="C1499" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1499" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1499" t="s">
         <v>2954</v>
       </c>
       <c r="O1499" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1499" t="s">
         <v>48</v>
       </c>
     </row>
@@ -43833,7 +43830,7 @@
         <v>104</v>
       </c>
       <c r="D1500" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1500" t="s">
         <v>2956</v>
@@ -43856,7 +43853,7 @@
         <v>104</v>
       </c>
       <c r="D1501" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1501" t="s">
         <v>2958</v>
@@ -43873,19 +43870,22 @@
         <v>2959</v>
       </c>
       <c r="B1502" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C1502" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D1502" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1502" t="s">
         <v>2960</v>
       </c>
       <c r="O1502" t="s">
-        <v>23</v>
+        <v>48</v>
+      </c>
+      <c r="P1502" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="1503">
@@ -43899,7 +43899,7 @@
         <v>20</v>
       </c>
       <c r="D1503" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1503" t="s">
         <v>2962</v>
@@ -43916,16 +43916,16 @@
         <v>113</v>
       </c>
       <c r="C1504" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D1504" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1504" t="s">
         <v>2964</v>
       </c>
       <c r="O1504" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1505">
@@ -43936,10 +43936,10 @@
         <v>113</v>
       </c>
       <c r="C1505" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D1505" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1505" t="s">
         <v>2966</v>
@@ -43956,10 +43956,10 @@
         <v>113</v>
       </c>
       <c r="C1506" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D1506" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1506" t="s">
         <v>2968</v>
@@ -43976,16 +43976,16 @@
         <v>113</v>
       </c>
       <c r="C1507" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1507" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1507" t="s">
         <v>2970</v>
       </c>
       <c r="O1507" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1508">
@@ -43999,7 +43999,7 @@
         <v>74</v>
       </c>
       <c r="D1508" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1508" t="s">
         <v>2972</v>
@@ -44019,7 +44019,7 @@
         <v>74</v>
       </c>
       <c r="D1509" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1509" t="s">
         <v>2974</v>
@@ -44036,16 +44036,16 @@
         <v>113</v>
       </c>
       <c r="C1510" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D1510" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1510" t="s">
         <v>2976</v>
       </c>
       <c r="O1510" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1511">
@@ -44056,10 +44056,10 @@
         <v>113</v>
       </c>
       <c r="C1511" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D1511" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1511" t="s">
         <v>2978</v>
@@ -44079,7 +44079,7 @@
         <v>95</v>
       </c>
       <c r="D1512" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1512" t="s">
         <v>2980</v>
@@ -44096,10 +44096,10 @@
         <v>113</v>
       </c>
       <c r="C1513" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1513" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1513" t="s">
         <v>2982</v>
@@ -44119,7 +44119,7 @@
         <v>104</v>
       </c>
       <c r="D1514" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1514" t="s">
         <v>2984</v>
@@ -44133,22 +44133,19 @@
         <v>2985</v>
       </c>
       <c r="B1515" t="s">
-        <v>2519</v>
+        <v>113</v>
       </c>
       <c r="C1515" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="D1515" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1515" t="s">
         <v>2986</v>
       </c>
       <c r="O1515" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1515" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1516">
@@ -44162,12 +44159,15 @@
         <v>74</v>
       </c>
       <c r="D1516" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1516" t="s">
         <v>2988</v>
       </c>
       <c r="O1516" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1516" t="s">
         <v>23</v>
       </c>
     </row>
@@ -44176,21 +44176,24 @@
         <v>2989</v>
       </c>
       <c r="B1517" t="s">
-        <v>19</v>
+        <v>2519</v>
       </c>
       <c r="C1517" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D1517" t="s">
-        <v>21</v>
+        <v>2939</v>
       </c>
       <c r="E1517" t="s">
-        <v>75</v>
+        <v>2990</v>
+      </c>
+      <c r="O1517" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1518">
       <c r="A1518" t="s">
-        <v>2990</v>
+        <v>2991</v>
       </c>
       <c r="B1518" t="s">
         <v>19</v>
@@ -44202,24 +44205,24 @@
         <v>21</v>
       </c>
       <c r="E1518" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="1519">
       <c r="A1519" t="s">
-        <v>2991</v>
+        <v>2992</v>
       </c>
       <c r="B1519" t="s">
         <v>19</v>
       </c>
       <c r="C1519" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="D1519" t="s">
         <v>21</v>
       </c>
       <c r="E1519" t="s">
-        <v>2992</v>
+        <v>70</v>
       </c>
     </row>
     <row r="1520">
@@ -44227,24 +44230,24 @@
         <v>2993</v>
       </c>
       <c r="B1520" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1520" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="D1520" t="s">
         <v>21</v>
       </c>
       <c r="E1520" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="1521">
       <c r="A1521" t="s">
+        <v>2995</v>
+      </c>
+      <c r="B1521" t="s">
         <v>2996</v>
-      </c>
-      <c r="B1521" t="s">
-        <v>2994</v>
       </c>
       <c r="C1521" t="s">
         <v>46</v>
@@ -44261,10 +44264,10 @@
         <v>2998</v>
       </c>
       <c r="B1522" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1522" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1522" t="s">
         <v>21</v>
@@ -44278,7 +44281,7 @@
         <v>3000</v>
       </c>
       <c r="B1523" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1523" t="s">
         <v>56</v>
@@ -44295,10 +44298,10 @@
         <v>3002</v>
       </c>
       <c r="B1524" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1524" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1524" t="s">
         <v>21</v>
@@ -44312,7 +44315,7 @@
         <v>3004</v>
       </c>
       <c r="B1525" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1525" t="s">
         <v>67</v>
@@ -44329,7 +44332,7 @@
         <v>3006</v>
       </c>
       <c r="B1526" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1526" t="s">
         <v>67</v>
@@ -44346,10 +44349,10 @@
         <v>3008</v>
       </c>
       <c r="B1527" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1527" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1527" t="s">
         <v>21</v>
@@ -44363,7 +44366,7 @@
         <v>3010</v>
       </c>
       <c r="B1528" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1528" t="s">
         <v>74</v>
@@ -44380,7 +44383,7 @@
         <v>3012</v>
       </c>
       <c r="B1529" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1529" t="s">
         <v>74</v>
@@ -44397,10 +44400,10 @@
         <v>3014</v>
       </c>
       <c r="B1530" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1530" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1530" t="s">
         <v>21</v>
@@ -44414,7 +44417,7 @@
         <v>3016</v>
       </c>
       <c r="B1531" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1531" t="s">
         <v>95</v>
@@ -44431,10 +44434,10 @@
         <v>3018</v>
       </c>
       <c r="B1532" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1532" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1532" t="s">
         <v>21</v>
@@ -44448,7 +44451,7 @@
         <v>3020</v>
       </c>
       <c r="B1533" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1533" t="s">
         <v>104</v>
@@ -44465,13 +44468,13 @@
         <v>3022</v>
       </c>
       <c r="B1534" t="s">
-        <v>19</v>
+        <v>2996</v>
       </c>
       <c r="C1534" t="s">
         <v>104</v>
       </c>
       <c r="D1534" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="E1534" t="s">
         <v>3023</v>
@@ -44482,10 +44485,10 @@
         <v>3024</v>
       </c>
       <c r="B1535" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1535" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="D1535" t="s">
         <v>195</v>
@@ -44499,7 +44502,7 @@
         <v>3026</v>
       </c>
       <c r="B1536" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1536" t="s">
         <v>56</v>
@@ -44516,10 +44519,10 @@
         <v>3028</v>
       </c>
       <c r="B1537" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1537" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D1537" t="s">
         <v>195</v>
@@ -44533,7 +44536,7 @@
         <v>3030</v>
       </c>
       <c r="B1538" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1538" t="s">
         <v>74</v>
@@ -44550,7 +44553,7 @@
         <v>3032</v>
       </c>
       <c r="B1539" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1539" t="s">
         <v>74</v>
@@ -44567,10 +44570,10 @@
         <v>3034</v>
       </c>
       <c r="B1540" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1540" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1540" t="s">
         <v>195</v>
@@ -44584,13 +44587,13 @@
         <v>3036</v>
       </c>
       <c r="B1541" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1541" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="D1541" t="s">
-        <v>349</v>
+        <v>195</v>
       </c>
       <c r="E1541" t="s">
         <v>3037</v>
@@ -44601,7 +44604,7 @@
         <v>3038</v>
       </c>
       <c r="B1542" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1542" t="s">
         <v>46</v>
@@ -44618,7 +44621,7 @@
         <v>3040</v>
       </c>
       <c r="B1543" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1543" t="s">
         <v>46</v>
@@ -44635,7 +44638,7 @@
         <v>3042</v>
       </c>
       <c r="B1544" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1544" t="s">
         <v>46</v>
@@ -44652,10 +44655,10 @@
         <v>3044</v>
       </c>
       <c r="B1545" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1545" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1545" t="s">
         <v>349</v>
@@ -44669,7 +44672,7 @@
         <v>3046</v>
       </c>
       <c r="B1546" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1546" t="s">
         <v>56</v>
@@ -44686,10 +44689,10 @@
         <v>3048</v>
       </c>
       <c r="B1547" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1547" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1547" t="s">
         <v>349</v>
@@ -44703,7 +44706,7 @@
         <v>3050</v>
       </c>
       <c r="B1548" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1548" t="s">
         <v>67</v>
@@ -44720,7 +44723,7 @@
         <v>3052</v>
       </c>
       <c r="B1549" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1549" t="s">
         <v>67</v>
@@ -44737,7 +44740,7 @@
         <v>3054</v>
       </c>
       <c r="B1550" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1550" t="s">
         <v>67</v>
@@ -44754,7 +44757,7 @@
         <v>3056</v>
       </c>
       <c r="B1551" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1551" t="s">
         <v>67</v>
@@ -44771,10 +44774,10 @@
         <v>3058</v>
       </c>
       <c r="B1552" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1552" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1552" t="s">
         <v>349</v>
@@ -44788,7 +44791,7 @@
         <v>3060</v>
       </c>
       <c r="B1553" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1553" t="s">
         <v>74</v>
@@ -44805,7 +44808,7 @@
         <v>3062</v>
       </c>
       <c r="B1554" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1554" t="s">
         <v>74</v>
@@ -44822,10 +44825,10 @@
         <v>3064</v>
       </c>
       <c r="B1555" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1555" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1555" t="s">
         <v>349</v>
@@ -44839,7 +44842,7 @@
         <v>3066</v>
       </c>
       <c r="B1556" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1556" t="s">
         <v>95</v>
@@ -44856,7 +44859,7 @@
         <v>3068</v>
       </c>
       <c r="B1557" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1557" t="s">
         <v>95</v>
@@ -44873,10 +44876,10 @@
         <v>3070</v>
       </c>
       <c r="B1558" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1558" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1558" t="s">
         <v>349</v>
@@ -44890,7 +44893,7 @@
         <v>3072</v>
       </c>
       <c r="B1559" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1559" t="s">
         <v>104</v>
@@ -44907,7 +44910,7 @@
         <v>3074</v>
       </c>
       <c r="B1560" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1560" t="s">
         <v>104</v>
@@ -44924,13 +44927,13 @@
         <v>3076</v>
       </c>
       <c r="B1561" t="s">
-        <v>19</v>
+        <v>2996</v>
       </c>
       <c r="C1561" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D1561" t="s">
-        <v>446</v>
+        <v>349</v>
       </c>
       <c r="E1561" t="s">
         <v>3077</v>
@@ -44941,10 +44944,10 @@
         <v>3078</v>
       </c>
       <c r="B1562" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1562" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="D1562" t="s">
         <v>446</v>
@@ -44958,7 +44961,7 @@
         <v>3080</v>
       </c>
       <c r="B1563" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1563" t="s">
         <v>67</v>
@@ -44975,10 +44978,10 @@
         <v>3082</v>
       </c>
       <c r="B1564" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1564" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1564" t="s">
         <v>446</v>
@@ -44992,7 +44995,7 @@
         <v>3084</v>
       </c>
       <c r="B1565" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1565" t="s">
         <v>74</v>
@@ -45009,7 +45012,7 @@
         <v>3086</v>
       </c>
       <c r="B1566" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1566" t="s">
         <v>74</v>
@@ -45026,10 +45029,10 @@
         <v>3088</v>
       </c>
       <c r="B1567" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1567" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1567" t="s">
         <v>446</v>
@@ -45043,7 +45046,7 @@
         <v>3090</v>
       </c>
       <c r="B1568" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1568" t="s">
         <v>95</v>
@@ -45060,7 +45063,7 @@
         <v>3092</v>
       </c>
       <c r="B1569" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1569" t="s">
         <v>95</v>
@@ -45077,7 +45080,7 @@
         <v>3094</v>
       </c>
       <c r="B1570" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1570" t="s">
         <v>95</v>
@@ -45094,10 +45097,10 @@
         <v>3096</v>
       </c>
       <c r="B1571" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1571" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1571" t="s">
         <v>446</v>
@@ -45111,7 +45114,7 @@
         <v>3098</v>
       </c>
       <c r="B1572" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1572" t="s">
         <v>104</v>
@@ -45128,7 +45131,7 @@
         <v>3100</v>
       </c>
       <c r="B1573" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1573" t="s">
         <v>104</v>
@@ -45145,7 +45148,7 @@
         <v>3102</v>
       </c>
       <c r="B1574" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1574" t="s">
         <v>104</v>
@@ -45162,13 +45165,13 @@
         <v>3104</v>
       </c>
       <c r="B1575" t="s">
-        <v>19</v>
+        <v>2996</v>
       </c>
       <c r="C1575" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1575" t="s">
-        <v>592</v>
+        <v>446</v>
       </c>
       <c r="E1575" t="s">
         <v>3105</v>
@@ -45182,18 +45185,18 @@
         <v>19</v>
       </c>
       <c r="C1576" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="D1576" t="s">
         <v>592</v>
       </c>
       <c r="E1576" t="s">
-        <v>3105</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="1577">
       <c r="A1577" t="s">
-        <v>3107</v>
+        <v>3108</v>
       </c>
       <c r="B1577" t="s">
         <v>19</v>
@@ -45205,41 +45208,41 @@
         <v>592</v>
       </c>
       <c r="E1577" t="s">
-        <v>2154</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="1578">
       <c r="A1578" t="s">
-        <v>3108</v>
+        <v>3109</v>
       </c>
       <c r="B1578" t="s">
         <v>19</v>
       </c>
       <c r="C1578" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D1578" t="s">
         <v>592</v>
       </c>
       <c r="E1578" t="s">
-        <v>3105</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="1579">
       <c r="A1579" t="s">
-        <v>3109</v>
+        <v>3110</v>
       </c>
       <c r="B1579" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1579" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1579" t="s">
         <v>592</v>
       </c>
       <c r="E1579" t="s">
-        <v>3110</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="1580">
@@ -45247,7 +45250,7 @@
         <v>3111</v>
       </c>
       <c r="B1580" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1580" t="s">
         <v>46</v>
@@ -45264,7 +45267,7 @@
         <v>3113</v>
       </c>
       <c r="B1581" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1581" t="s">
         <v>46</v>
@@ -45281,10 +45284,10 @@
         <v>3115</v>
       </c>
       <c r="B1582" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1582" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1582" t="s">
         <v>592</v>
@@ -45298,7 +45301,7 @@
         <v>3117</v>
       </c>
       <c r="B1583" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1583" t="s">
         <v>56</v>
@@ -45315,10 +45318,10 @@
         <v>3119</v>
       </c>
       <c r="B1584" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1584" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1584" t="s">
         <v>592</v>
@@ -45332,7 +45335,7 @@
         <v>3121</v>
       </c>
       <c r="B1585" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1585" t="s">
         <v>67</v>
@@ -45349,7 +45352,7 @@
         <v>3123</v>
       </c>
       <c r="B1586" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1586" t="s">
         <v>67</v>
@@ -45366,7 +45369,7 @@
         <v>3125</v>
       </c>
       <c r="B1587" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1587" t="s">
         <v>67</v>
@@ -45383,10 +45386,10 @@
         <v>3127</v>
       </c>
       <c r="B1588" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1588" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1588" t="s">
         <v>592</v>
@@ -45400,7 +45403,7 @@
         <v>3129</v>
       </c>
       <c r="B1589" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1589" t="s">
         <v>74</v>
@@ -45417,7 +45420,7 @@
         <v>3131</v>
       </c>
       <c r="B1590" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1590" t="s">
         <v>74</v>
@@ -45434,7 +45437,7 @@
         <v>3133</v>
       </c>
       <c r="B1591" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1591" t="s">
         <v>74</v>
@@ -45451,7 +45454,7 @@
         <v>3135</v>
       </c>
       <c r="B1592" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1592" t="s">
         <v>74</v>
@@ -45468,7 +45471,7 @@
         <v>3137</v>
       </c>
       <c r="B1593" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1593" t="s">
         <v>74</v>
@@ -45485,10 +45488,10 @@
         <v>3139</v>
       </c>
       <c r="B1594" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1594" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1594" t="s">
         <v>592</v>
@@ -45502,7 +45505,7 @@
         <v>3141</v>
       </c>
       <c r="B1595" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1595" t="s">
         <v>95</v>
@@ -45519,10 +45522,10 @@
         <v>3143</v>
       </c>
       <c r="B1596" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1596" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1596" t="s">
         <v>592</v>
@@ -45536,13 +45539,13 @@
         <v>3145</v>
       </c>
       <c r="B1597" t="s">
-        <v>19</v>
+        <v>2996</v>
       </c>
       <c r="C1597" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1597" t="s">
-        <v>769</v>
+        <v>592</v>
       </c>
       <c r="E1597" t="s">
         <v>3146</v>
@@ -45553,7 +45556,7 @@
         <v>3147</v>
       </c>
       <c r="B1598" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1598" t="s">
         <v>46</v>
@@ -45570,7 +45573,7 @@
         <v>3149</v>
       </c>
       <c r="B1599" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1599" t="s">
         <v>46</v>
@@ -45587,7 +45590,7 @@
         <v>3151</v>
       </c>
       <c r="B1600" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1600" t="s">
         <v>46</v>
@@ -45604,7 +45607,7 @@
         <v>3153</v>
       </c>
       <c r="B1601" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1601" t="s">
         <v>46</v>
@@ -45621,10 +45624,10 @@
         <v>3155</v>
       </c>
       <c r="B1602" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1602" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1602" t="s">
         <v>769</v>
@@ -45638,10 +45641,10 @@
         <v>3157</v>
       </c>
       <c r="B1603" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1603" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D1603" t="s">
         <v>769</v>
@@ -45655,7 +45658,7 @@
         <v>3159</v>
       </c>
       <c r="B1604" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1604" t="s">
         <v>74</v>
@@ -45672,7 +45675,7 @@
         <v>3161</v>
       </c>
       <c r="B1605" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1605" t="s">
         <v>74</v>
@@ -45689,7 +45692,7 @@
         <v>3163</v>
       </c>
       <c r="B1606" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1606" t="s">
         <v>74</v>
@@ -45706,10 +45709,10 @@
         <v>3165</v>
       </c>
       <c r="B1607" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1607" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1607" t="s">
         <v>769</v>
@@ -45723,7 +45726,7 @@
         <v>3167</v>
       </c>
       <c r="B1608" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1608" t="s">
         <v>95</v>
@@ -45740,10 +45743,10 @@
         <v>3169</v>
       </c>
       <c r="B1609" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1609" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1609" t="s">
         <v>769</v>
@@ -45757,7 +45760,7 @@
         <v>3171</v>
       </c>
       <c r="B1610" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1610" t="s">
         <v>104</v>
@@ -45774,13 +45777,13 @@
         <v>3173</v>
       </c>
       <c r="B1611" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1611" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1611" t="s">
-        <v>909</v>
+        <v>769</v>
       </c>
       <c r="E1611" t="s">
         <v>3174</v>
@@ -45791,7 +45794,7 @@
         <v>3175</v>
       </c>
       <c r="B1612" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1612" t="s">
         <v>46</v>
@@ -45808,7 +45811,7 @@
         <v>3177</v>
       </c>
       <c r="B1613" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1613" t="s">
         <v>46</v>
@@ -45825,10 +45828,10 @@
         <v>3179</v>
       </c>
       <c r="B1614" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1614" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1614" t="s">
         <v>909</v>
@@ -45842,10 +45845,10 @@
         <v>3181</v>
       </c>
       <c r="B1615" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1615" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D1615" t="s">
         <v>909</v>
@@ -45859,7 +45862,7 @@
         <v>3183</v>
       </c>
       <c r="B1616" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1616" t="s">
         <v>74</v>
@@ -45876,10 +45879,10 @@
         <v>3185</v>
       </c>
       <c r="B1617" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1617" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1617" t="s">
         <v>909</v>
@@ -45893,7 +45896,7 @@
         <v>3187</v>
       </c>
       <c r="B1618" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1618" t="s">
         <v>95</v>
@@ -45910,7 +45913,7 @@
         <v>3189</v>
       </c>
       <c r="B1619" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1619" t="s">
         <v>95</v>
@@ -45927,10 +45930,10 @@
         <v>3191</v>
       </c>
       <c r="B1620" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1620" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1620" t="s">
         <v>909</v>
@@ -45944,7 +45947,7 @@
         <v>3193</v>
       </c>
       <c r="B1621" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1621" t="s">
         <v>104</v>
@@ -45961,7 +45964,7 @@
         <v>3195</v>
       </c>
       <c r="B1622" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1622" t="s">
         <v>104</v>
@@ -45978,13 +45981,13 @@
         <v>3197</v>
       </c>
       <c r="B1623" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1623" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1623" t="s">
-        <v>1059</v>
+        <v>909</v>
       </c>
       <c r="E1623" t="s">
         <v>3198</v>
@@ -45995,10 +45998,10 @@
         <v>3199</v>
       </c>
       <c r="B1624" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1624" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1624" t="s">
         <v>1059</v>
@@ -46012,10 +46015,10 @@
         <v>3201</v>
       </c>
       <c r="B1625" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1625" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1625" t="s">
         <v>1059</v>
@@ -46029,7 +46032,7 @@
         <v>3203</v>
       </c>
       <c r="B1626" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1626" t="s">
         <v>67</v>
@@ -46046,7 +46049,7 @@
         <v>3205</v>
       </c>
       <c r="B1627" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1627" t="s">
         <v>67</v>
@@ -46063,7 +46066,7 @@
         <v>3207</v>
       </c>
       <c r="B1628" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1628" t="s">
         <v>67</v>
@@ -46080,10 +46083,10 @@
         <v>3209</v>
       </c>
       <c r="B1629" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1629" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1629" t="s">
         <v>1059</v>
@@ -46097,7 +46100,7 @@
         <v>3211</v>
       </c>
       <c r="B1630" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1630" t="s">
         <v>74</v>
@@ -46114,7 +46117,7 @@
         <v>3213</v>
       </c>
       <c r="B1631" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1631" t="s">
         <v>74</v>
@@ -46131,10 +46134,10 @@
         <v>3215</v>
       </c>
       <c r="B1632" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1632" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1632" t="s">
         <v>1059</v>
@@ -46148,7 +46151,7 @@
         <v>3217</v>
       </c>
       <c r="B1633" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1633" t="s">
         <v>95</v>
@@ -46165,10 +46168,10 @@
         <v>3219</v>
       </c>
       <c r="B1634" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1634" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1634" t="s">
         <v>1059</v>
@@ -46182,33 +46185,33 @@
         <v>3221</v>
       </c>
       <c r="B1635" t="s">
-        <v>19</v>
+        <v>2996</v>
       </c>
       <c r="C1635" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D1635" t="s">
-        <v>1191</v>
+        <v>1059</v>
       </c>
       <c r="E1635" t="s">
-        <v>1248</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="1636">
       <c r="A1636" t="s">
-        <v>3222</v>
+        <v>3223</v>
       </c>
       <c r="B1636" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1636" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="D1636" t="s">
         <v>1191</v>
       </c>
       <c r="E1636" t="s">
-        <v>3223</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1637">
@@ -46216,7 +46219,7 @@
         <v>3224</v>
       </c>
       <c r="B1637" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1637" t="s">
         <v>46</v>
@@ -46233,7 +46236,7 @@
         <v>3226</v>
       </c>
       <c r="B1638" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1638" t="s">
         <v>46</v>
@@ -46250,7 +46253,7 @@
         <v>3228</v>
       </c>
       <c r="B1639" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1639" t="s">
         <v>46</v>
@@ -46267,7 +46270,7 @@
         <v>3230</v>
       </c>
       <c r="B1640" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1640" t="s">
         <v>46</v>
@@ -46284,7 +46287,7 @@
         <v>3232</v>
       </c>
       <c r="B1641" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1641" t="s">
         <v>46</v>
@@ -46301,7 +46304,7 @@
         <v>3234</v>
       </c>
       <c r="B1642" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1642" t="s">
         <v>46</v>
@@ -46318,10 +46321,10 @@
         <v>3236</v>
       </c>
       <c r="B1643" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1643" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1643" t="s">
         <v>1191</v>
@@ -46335,10 +46338,10 @@
         <v>3238</v>
       </c>
       <c r="B1644" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1644" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1644" t="s">
         <v>1191</v>
@@ -46352,7 +46355,7 @@
         <v>3240</v>
       </c>
       <c r="B1645" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1645" t="s">
         <v>67</v>
@@ -46369,10 +46372,10 @@
         <v>3242</v>
       </c>
       <c r="B1646" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1646" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1646" t="s">
         <v>1191</v>
@@ -46386,10 +46389,10 @@
         <v>3244</v>
       </c>
       <c r="B1647" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1647" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1647" t="s">
         <v>1191</v>
@@ -46403,7 +46406,7 @@
         <v>3246</v>
       </c>
       <c r="B1648" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1648" t="s">
         <v>95</v>
@@ -46420,7 +46423,7 @@
         <v>3248</v>
       </c>
       <c r="B1649" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1649" t="s">
         <v>95</v>
@@ -46437,7 +46440,7 @@
         <v>3250</v>
       </c>
       <c r="B1650" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1650" t="s">
         <v>95</v>
@@ -46454,10 +46457,10 @@
         <v>3252</v>
       </c>
       <c r="B1651" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1651" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1651" t="s">
         <v>1191</v>
@@ -46471,7 +46474,7 @@
         <v>3254</v>
       </c>
       <c r="B1652" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1652" t="s">
         <v>104</v>
@@ -46488,7 +46491,7 @@
         <v>3256</v>
       </c>
       <c r="B1653" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1653" t="s">
         <v>104</v>
@@ -46505,7 +46508,7 @@
         <v>3258</v>
       </c>
       <c r="B1654" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1654" t="s">
         <v>104</v>
@@ -46522,13 +46525,13 @@
         <v>3260</v>
       </c>
       <c r="B1655" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1655" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1655" t="s">
-        <v>1341</v>
+        <v>1191</v>
       </c>
       <c r="E1655" t="s">
         <v>3261</v>
@@ -46539,7 +46542,7 @@
         <v>3262</v>
       </c>
       <c r="B1656" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1656" t="s">
         <v>46</v>
@@ -46556,10 +46559,10 @@
         <v>3264</v>
       </c>
       <c r="B1657" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1657" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1657" t="s">
         <v>1341</v>
@@ -46573,7 +46576,7 @@
         <v>3266</v>
       </c>
       <c r="B1658" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1658" t="s">
         <v>56</v>
@@ -46590,10 +46593,10 @@
         <v>3268</v>
       </c>
       <c r="B1659" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1659" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1659" t="s">
         <v>1341</v>
@@ -46607,7 +46610,7 @@
         <v>3270</v>
       </c>
       <c r="B1660" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1660" t="s">
         <v>67</v>
@@ -46624,7 +46627,7 @@
         <v>3272</v>
       </c>
       <c r="B1661" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1661" t="s">
         <v>67</v>
@@ -46641,10 +46644,10 @@
         <v>3274</v>
       </c>
       <c r="B1662" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1662" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1662" t="s">
         <v>1341</v>
@@ -46658,7 +46661,7 @@
         <v>3276</v>
       </c>
       <c r="B1663" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1663" t="s">
         <v>74</v>
@@ -46675,10 +46678,10 @@
         <v>3278</v>
       </c>
       <c r="B1664" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1664" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1664" t="s">
         <v>1341</v>
@@ -46692,7 +46695,7 @@
         <v>3280</v>
       </c>
       <c r="B1665" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1665" t="s">
         <v>95</v>
@@ -46709,7 +46712,7 @@
         <v>3282</v>
       </c>
       <c r="B1666" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1666" t="s">
         <v>95</v>
@@ -46726,10 +46729,10 @@
         <v>3284</v>
       </c>
       <c r="B1667" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1667" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1667" t="s">
         <v>1341</v>
@@ -46743,7 +46746,7 @@
         <v>3286</v>
       </c>
       <c r="B1668" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1668" t="s">
         <v>104</v>
@@ -46760,7 +46763,7 @@
         <v>3288</v>
       </c>
       <c r="B1669" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1669" t="s">
         <v>104</v>
@@ -46777,13 +46780,13 @@
         <v>3290</v>
       </c>
       <c r="B1670" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1670" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1670" t="s">
-        <v>1467</v>
+        <v>1341</v>
       </c>
       <c r="E1670" t="s">
         <v>3291</v>
@@ -46794,7 +46797,7 @@
         <v>3292</v>
       </c>
       <c r="B1671" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1671" t="s">
         <v>46</v>
@@ -46811,7 +46814,7 @@
         <v>3294</v>
       </c>
       <c r="B1672" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1672" t="s">
         <v>46</v>
@@ -46828,7 +46831,7 @@
         <v>3296</v>
       </c>
       <c r="B1673" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1673" t="s">
         <v>46</v>
@@ -46845,7 +46848,7 @@
         <v>3298</v>
       </c>
       <c r="B1674" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1674" t="s">
         <v>46</v>
@@ -46862,7 +46865,7 @@
         <v>3300</v>
       </c>
       <c r="B1675" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1675" t="s">
         <v>46</v>
@@ -46879,10 +46882,10 @@
         <v>3302</v>
       </c>
       <c r="B1676" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1676" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1676" t="s">
         <v>1467</v>
@@ -46896,7 +46899,7 @@
         <v>3304</v>
       </c>
       <c r="B1677" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1677" t="s">
         <v>56</v>
@@ -46913,7 +46916,7 @@
         <v>3306</v>
       </c>
       <c r="B1678" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1678" t="s">
         <v>56</v>
@@ -46930,10 +46933,10 @@
         <v>3308</v>
       </c>
       <c r="B1679" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1679" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1679" t="s">
         <v>1467</v>
@@ -46947,7 +46950,7 @@
         <v>3310</v>
       </c>
       <c r="B1680" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1680" t="s">
         <v>67</v>
@@ -46964,10 +46967,10 @@
         <v>3312</v>
       </c>
       <c r="B1681" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1681" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1681" t="s">
         <v>1467</v>
@@ -46981,7 +46984,7 @@
         <v>3314</v>
       </c>
       <c r="B1682" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1682" t="s">
         <v>74</v>
@@ -46998,7 +47001,7 @@
         <v>3316</v>
       </c>
       <c r="B1683" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1683" t="s">
         <v>74</v>
@@ -47015,7 +47018,7 @@
         <v>3318</v>
       </c>
       <c r="B1684" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1684" t="s">
         <v>74</v>
@@ -47032,7 +47035,7 @@
         <v>3320</v>
       </c>
       <c r="B1685" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1685" t="s">
         <v>74</v>
@@ -47049,7 +47052,7 @@
         <v>3322</v>
       </c>
       <c r="B1686" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1686" t="s">
         <v>74</v>
@@ -47066,7 +47069,7 @@
         <v>3324</v>
       </c>
       <c r="B1687" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1687" t="s">
         <v>74</v>
@@ -47083,10 +47086,10 @@
         <v>3326</v>
       </c>
       <c r="B1688" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1688" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1688" t="s">
         <v>1467</v>
@@ -47100,7 +47103,7 @@
         <v>3328</v>
       </c>
       <c r="B1689" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1689" t="s">
         <v>95</v>
@@ -47117,7 +47120,7 @@
         <v>3330</v>
       </c>
       <c r="B1690" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1690" t="s">
         <v>95</v>
@@ -47134,7 +47137,7 @@
         <v>3332</v>
       </c>
       <c r="B1691" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1691" t="s">
         <v>95</v>
@@ -47151,7 +47154,7 @@
         <v>3334</v>
       </c>
       <c r="B1692" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1692" t="s">
         <v>95</v>
@@ -47168,7 +47171,7 @@
         <v>3336</v>
       </c>
       <c r="B1693" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1693" t="s">
         <v>95</v>
@@ -47185,10 +47188,10 @@
         <v>3338</v>
       </c>
       <c r="B1694" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1694" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1694" t="s">
         <v>1467</v>
@@ -47202,7 +47205,7 @@
         <v>3340</v>
       </c>
       <c r="B1695" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1695" t="s">
         <v>104</v>
@@ -47219,7 +47222,7 @@
         <v>3342</v>
       </c>
       <c r="B1696" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1696" t="s">
         <v>104</v>
@@ -47236,7 +47239,7 @@
         <v>3344</v>
       </c>
       <c r="B1697" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1697" t="s">
         <v>104</v>
@@ -47253,13 +47256,13 @@
         <v>3346</v>
       </c>
       <c r="B1698" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1698" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1698" t="s">
-        <v>1555</v>
+        <v>1467</v>
       </c>
       <c r="E1698" t="s">
         <v>3347</v>
@@ -47270,10 +47273,10 @@
         <v>3348</v>
       </c>
       <c r="B1699" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1699" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D1699" t="s">
         <v>1555</v>
@@ -47287,10 +47290,10 @@
         <v>3350</v>
       </c>
       <c r="B1700" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1700" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1700" t="s">
         <v>1555</v>
@@ -47304,7 +47307,7 @@
         <v>3352</v>
       </c>
       <c r="B1701" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1701" t="s">
         <v>74</v>
@@ -47321,7 +47324,7 @@
         <v>3354</v>
       </c>
       <c r="B1702" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1702" t="s">
         <v>74</v>
@@ -47338,10 +47341,10 @@
         <v>3356</v>
       </c>
       <c r="B1703" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1703" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D1703" t="s">
         <v>1555</v>
@@ -47355,7 +47358,7 @@
         <v>3358</v>
       </c>
       <c r="B1704" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1704" t="s">
         <v>104</v>
@@ -47372,7 +47375,7 @@
         <v>3360</v>
       </c>
       <c r="B1705" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1705" t="s">
         <v>104</v>
@@ -47389,33 +47392,33 @@
         <v>3362</v>
       </c>
       <c r="B1706" t="s">
-        <v>19</v>
+        <v>2996</v>
       </c>
       <c r="C1706" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D1706" t="s">
-        <v>1674</v>
+        <v>1555</v>
       </c>
       <c r="E1706" t="s">
-        <v>1586</v>
+        <v>3363</v>
       </c>
     </row>
     <row r="1707">
       <c r="A1707" t="s">
-        <v>3363</v>
+        <v>3364</v>
       </c>
       <c r="B1707" t="s">
-        <v>2994</v>
+        <v>19</v>
       </c>
       <c r="C1707" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="D1707" t="s">
         <v>1674</v>
       </c>
       <c r="E1707" t="s">
-        <v>3364</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1708">
@@ -47423,10 +47426,10 @@
         <v>3365</v>
       </c>
       <c r="B1708" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1708" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1708" t="s">
         <v>1674</v>
@@ -47440,10 +47443,10 @@
         <v>3367</v>
       </c>
       <c r="B1709" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1709" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1709" t="s">
         <v>1674</v>
@@ -47457,7 +47460,7 @@
         <v>3369</v>
       </c>
       <c r="B1710" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1710" t="s">
         <v>67</v>
@@ -47474,10 +47477,10 @@
         <v>3371</v>
       </c>
       <c r="B1711" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1711" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1711" t="s">
         <v>1674</v>
@@ -47491,7 +47494,7 @@
         <v>3373</v>
       </c>
       <c r="B1712" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1712" t="s">
         <v>74</v>
@@ -47508,10 +47511,10 @@
         <v>3375</v>
       </c>
       <c r="B1713" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1713" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1713" t="s">
         <v>1674</v>
@@ -47525,7 +47528,7 @@
         <v>3377</v>
       </c>
       <c r="B1714" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1714" t="s">
         <v>95</v>
@@ -47542,7 +47545,7 @@
         <v>3379</v>
       </c>
       <c r="B1715" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1715" t="s">
         <v>95</v>
@@ -47559,10 +47562,10 @@
         <v>3381</v>
       </c>
       <c r="B1716" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1716" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1716" t="s">
         <v>1674</v>
@@ -47576,7 +47579,7 @@
         <v>3383</v>
       </c>
       <c r="B1717" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1717" t="s">
         <v>104</v>
@@ -47593,13 +47596,13 @@
         <v>3385</v>
       </c>
       <c r="B1718" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1718" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1718" t="s">
-        <v>1775</v>
+        <v>1674</v>
       </c>
       <c r="E1718" t="s">
         <v>3386</v>
@@ -47610,10 +47613,10 @@
         <v>3387</v>
       </c>
       <c r="B1719" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1719" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1719" t="s">
         <v>1775</v>
@@ -47627,7 +47630,7 @@
         <v>3389</v>
       </c>
       <c r="B1720" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1720" t="s">
         <v>56</v>
@@ -47644,10 +47647,10 @@
         <v>3391</v>
       </c>
       <c r="B1721" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1721" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1721" t="s">
         <v>1775</v>
@@ -47661,7 +47664,7 @@
         <v>3393</v>
       </c>
       <c r="B1722" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1722" t="s">
         <v>67</v>
@@ -47678,10 +47681,10 @@
         <v>3395</v>
       </c>
       <c r="B1723" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1723" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="D1723" t="s">
         <v>1775</v>
@@ -47695,7 +47698,7 @@
         <v>3397</v>
       </c>
       <c r="B1724" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1724" t="s">
         <v>95</v>
@@ -47712,7 +47715,7 @@
         <v>3399</v>
       </c>
       <c r="B1725" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1725" t="s">
         <v>95</v>
@@ -47729,7 +47732,7 @@
         <v>3401</v>
       </c>
       <c r="B1726" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1726" t="s">
         <v>95</v>
@@ -47746,10 +47749,10 @@
         <v>3403</v>
       </c>
       <c r="B1727" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1727" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1727" t="s">
         <v>1775</v>
@@ -47763,13 +47766,13 @@
         <v>3405</v>
       </c>
       <c r="B1728" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1728" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D1728" t="s">
-        <v>1872</v>
+        <v>1775</v>
       </c>
       <c r="E1728" t="s">
         <v>3406</v>
@@ -47780,7 +47783,7 @@
         <v>3407</v>
       </c>
       <c r="B1729" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1729" t="s">
         <v>46</v>
@@ -47797,7 +47800,7 @@
         <v>3409</v>
       </c>
       <c r="B1730" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1730" t="s">
         <v>46</v>
@@ -47814,7 +47817,7 @@
         <v>3411</v>
       </c>
       <c r="B1731" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1731" t="s">
         <v>46</v>
@@ -47831,7 +47834,7 @@
         <v>3413</v>
       </c>
       <c r="B1732" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1732" t="s">
         <v>46</v>
@@ -47848,10 +47851,10 @@
         <v>3415</v>
       </c>
       <c r="B1733" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1733" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D1733" t="s">
         <v>1872</v>
@@ -47865,10 +47868,10 @@
         <v>3417</v>
       </c>
       <c r="B1734" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1734" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1734" t="s">
         <v>1872</v>
@@ -47882,7 +47885,7 @@
         <v>3419</v>
       </c>
       <c r="B1735" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1735" t="s">
         <v>67</v>
@@ -47899,7 +47902,7 @@
         <v>3421</v>
       </c>
       <c r="B1736" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1736" t="s">
         <v>67</v>
@@ -47916,7 +47919,7 @@
         <v>3423</v>
       </c>
       <c r="B1737" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1737" t="s">
         <v>67</v>
@@ -47933,7 +47936,7 @@
         <v>3425</v>
       </c>
       <c r="B1738" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1738" t="s">
         <v>67</v>
@@ -47950,10 +47953,10 @@
         <v>3427</v>
       </c>
       <c r="B1739" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1739" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D1739" t="s">
         <v>1872</v>
@@ -47967,7 +47970,7 @@
         <v>3429</v>
       </c>
       <c r="B1740" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1740" t="s">
         <v>74</v>
@@ -47984,7 +47987,7 @@
         <v>3431</v>
       </c>
       <c r="B1741" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1741" t="s">
         <v>74</v>
@@ -48001,10 +48004,10 @@
         <v>3433</v>
       </c>
       <c r="B1742" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1742" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1742" t="s">
         <v>1872</v>
@@ -48018,7 +48021,7 @@
         <v>3435</v>
       </c>
       <c r="B1743" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1743" t="s">
         <v>95</v>
@@ -48035,7 +48038,7 @@
         <v>3437</v>
       </c>
       <c r="B1744" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1744" t="s">
         <v>95</v>
@@ -48052,7 +48055,7 @@
         <v>3439</v>
       </c>
       <c r="B1745" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1745" t="s">
         <v>95</v>
@@ -48069,10 +48072,10 @@
         <v>3441</v>
       </c>
       <c r="B1746" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1746" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1746" t="s">
         <v>1872</v>
@@ -48086,7 +48089,7 @@
         <v>3443</v>
       </c>
       <c r="B1747" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1747" t="s">
         <v>104</v>
@@ -48103,7 +48106,7 @@
         <v>3445</v>
       </c>
       <c r="B1748" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1748" t="s">
         <v>104</v>
@@ -48120,7 +48123,7 @@
         <v>3447</v>
       </c>
       <c r="B1749" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1749" t="s">
         <v>104</v>
@@ -48137,7 +48140,7 @@
         <v>3449</v>
       </c>
       <c r="B1750" t="s">
-        <v>2994</v>
+        <v>2996</v>
       </c>
       <c r="C1750" t="s">
         <v>104</v>
@@ -48154,13 +48157,13 @@
         <v>3451</v>
       </c>
       <c r="B1751" t="s">
-        <v>113</v>
+        <v>2996</v>
       </c>
       <c r="C1751" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D1751" t="s">
-        <v>2131</v>
+        <v>1872</v>
       </c>
       <c r="E1751" t="s">
         <v>3452</v>
@@ -48174,7 +48177,7 @@
         <v>113</v>
       </c>
       <c r="C1752" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="D1752" t="s">
         <v>2131</v>
@@ -48188,24 +48191,24 @@
         <v>3455</v>
       </c>
       <c r="B1753" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="C1753" t="s">
         <v>104</v>
       </c>
       <c r="D1753" t="s">
-        <v>2241</v>
+        <v>2131</v>
       </c>
       <c r="E1753" t="s">
-        <v>2244</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="1754">
       <c r="A1754" t="s">
-        <v>3456</v>
+        <v>3457</v>
       </c>
       <c r="B1754" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C1754" t="s">
         <v>104</v>
@@ -48214,7 +48217,7 @@
         <v>2241</v>
       </c>
       <c r="E1754" t="s">
-        <v>3457</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="1755">
@@ -48225,10 +48228,10 @@
         <v>113</v>
       </c>
       <c r="C1755" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D1755" t="s">
-        <v>2329</v>
+        <v>2241</v>
       </c>
       <c r="E1755" t="s">
         <v>3459</v>
@@ -48242,30 +48245,30 @@
         <v>113</v>
       </c>
       <c r="C1756" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="D1756" t="s">
         <v>2329</v>
       </c>
       <c r="E1756" t="s">
-        <v>3459</v>
+        <v>3461</v>
       </c>
     </row>
     <row r="1757">
       <c r="A1757" t="s">
-        <v>3461</v>
+        <v>3462</v>
       </c>
       <c r="B1757" t="s">
         <v>113</v>
       </c>
       <c r="C1757" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D1757" t="s">
         <v>2329</v>
       </c>
       <c r="E1757" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
     </row>
     <row r="1758">
@@ -48276,7 +48279,7 @@
         <v>113</v>
       </c>
       <c r="C1758" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D1758" t="s">
         <v>2329</v>
@@ -48290,13 +48293,13 @@
         <v>3465</v>
       </c>
       <c r="B1759" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="C1759" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D1759" t="s">
-        <v>2526</v>
+        <v>2329</v>
       </c>
       <c r="E1759" t="s">
         <v>3466</v>
@@ -48310,7 +48313,7 @@
         <v>19</v>
       </c>
       <c r="C1760" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="D1760" t="s">
         <v>2526</v>
@@ -48327,18 +48330,18 @@
         <v>19</v>
       </c>
       <c r="C1761" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D1761" t="s">
         <v>2526</v>
       </c>
       <c r="E1761" t="s">
-        <v>3468</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="1762">
       <c r="A1762" t="s">
-        <v>3470</v>
+        <v>3471</v>
       </c>
       <c r="B1762" t="s">
         <v>19</v>
@@ -48347,10 +48350,10 @@
         <v>104</v>
       </c>
       <c r="D1762" t="s">
-        <v>2648</v>
+        <v>2526</v>
       </c>
       <c r="E1762" t="s">
-        <v>3471</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="1763">
@@ -48358,67 +48361,67 @@
         <v>3472</v>
       </c>
       <c r="B1763" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C1763" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="D1763" t="s">
         <v>2648</v>
       </c>
       <c r="E1763" t="s">
-        <v>2685</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="1764">
       <c r="A1764" t="s">
-        <v>3473</v>
+        <v>3474</v>
       </c>
       <c r="B1764" t="s">
         <v>113</v>
       </c>
       <c r="C1764" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D1764" t="s">
         <v>2648</v>
       </c>
       <c r="E1764" t="s">
-        <v>2632</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="1765">
       <c r="A1765" t="s">
-        <v>3474</v>
+        <v>3475</v>
       </c>
       <c r="B1765" t="s">
         <v>113</v>
       </c>
       <c r="C1765" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="D1765" t="s">
         <v>2648</v>
       </c>
       <c r="E1765" t="s">
-        <v>2685</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="1766">
       <c r="A1766" t="s">
-        <v>3475</v>
+        <v>3476</v>
       </c>
       <c r="B1766" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="C1766" t="s">
         <v>104</v>
       </c>
       <c r="D1766" t="s">
-        <v>2873</v>
+        <v>2648</v>
       </c>
       <c r="E1766" t="s">
-        <v>3476</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="1767">
@@ -48432,7 +48435,7 @@
         <v>46</v>
       </c>
       <c r="D1767" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1767" t="s">
         <v>2878</v>
@@ -48449,10 +48452,10 @@
         <v>74</v>
       </c>
       <c r="D1768" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1768" t="s">
-        <v>2942</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="1769">
@@ -48466,7 +48469,7 @@
         <v>95</v>
       </c>
       <c r="D1769" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1769" t="s">
         <v>3480</v>
@@ -48483,7 +48486,7 @@
         <v>104</v>
       </c>
       <c r="D1770" t="s">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="E1770" t="s">
         <v>3482</v>

</xml_diff>

<commit_message>
Add: stickyheadersrecyclerview to show headers on lineuplist; Add: CalendarFragment now forces viewmodel with current day on a fragment creation, needs to make lineup list filled; Add: LineupAdapter migrated to a new adapter type with headers support;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11442" uniqueCount="3483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11439" uniqueCount="3483">
   <si>
     <t>Vehicles</t>
   </si>
@@ -20832,9 +20832,6 @@
       <c r="H473" t="s">
         <v>23</v>
       </c>
-      <c r="L473" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="474">
       <c r="A474" t="s">
@@ -22456,9 +22453,6 @@
       <c r="K544" t="s">
         <v>48</v>
       </c>
-      <c r="L544" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="545">
       <c r="A545" t="s">
@@ -24050,9 +24044,6 @@
         <v>48</v>
       </c>
       <c r="K613" t="s">
-        <v>48</v>
-      </c>
-      <c r="L613" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: Sticky headers and favorite list for vehicleList;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10345" uniqueCount="3035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10316" uniqueCount="3035">
   <si>
     <t>Vehicles</t>
   </si>
@@ -12014,9 +12014,6 @@
       <c r="F138" t="s">
         <v>48</v>
       </c>
-      <c r="G138" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
@@ -14359,9 +14356,6 @@
       <c r="G247" t="s">
         <v>48</v>
       </c>
-      <c r="H247" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
@@ -15098,9 +15092,6 @@
       <c r="G279" t="s">
         <v>23</v>
       </c>
-      <c r="H279" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
@@ -16177,9 +16168,6 @@
       <c r="E328" t="s">
         <v>667</v>
       </c>
-      <c r="F328" t="s">
-        <v>48</v>
-      </c>
       <c r="G328" t="s">
         <v>48</v>
       </c>
@@ -16209,9 +16197,6 @@
       <c r="H329" t="s">
         <v>48</v>
       </c>
-      <c r="I329" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="330">
       <c r="A330" t="s">
@@ -16390,9 +16375,6 @@
       <c r="E337" t="s">
         <v>667</v>
       </c>
-      <c r="F337" t="s">
-        <v>48</v>
-      </c>
       <c r="G337" t="s">
         <v>48</v>
       </c>
@@ -17267,9 +17249,6 @@
       <c r="E375" t="s">
         <v>755</v>
       </c>
-      <c r="F375" t="s">
-        <v>23</v>
-      </c>
       <c r="G375" t="s">
         <v>23</v>
       </c>
@@ -18040,9 +18019,6 @@
       <c r="H409" t="s">
         <v>48</v>
       </c>
-      <c r="I409" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="410">
       <c r="A410" t="s">
@@ -19827,9 +19803,6 @@
       <c r="E488" t="s">
         <v>973</v>
       </c>
-      <c r="G488" t="s">
-        <v>48</v>
-      </c>
       <c r="H488" t="s">
         <v>48</v>
       </c>
@@ -19853,9 +19826,6 @@
       <c r="E489" t="s">
         <v>975</v>
       </c>
-      <c r="G489" t="s">
-        <v>48</v>
-      </c>
       <c r="H489" t="s">
         <v>48</v>
       </c>
@@ -20250,9 +20220,6 @@
       <c r="E506" t="s">
         <v>1007</v>
       </c>
-      <c r="G506" t="s">
-        <v>23</v>
-      </c>
       <c r="H506" t="s">
         <v>23</v>
       </c>
@@ -20529,9 +20496,6 @@
       <c r="E518" t="s">
         <v>1031</v>
       </c>
-      <c r="G518" t="s">
-        <v>23</v>
-      </c>
       <c r="H518" t="s">
         <v>23</v>
       </c>
@@ -22039,9 +22003,6 @@
       <c r="E583" t="s">
         <v>1156</v>
       </c>
-      <c r="G583" t="s">
-        <v>23</v>
-      </c>
       <c r="H583" t="s">
         <v>23</v>
       </c>
@@ -22252,9 +22213,6 @@
       <c r="E592" t="s">
         <v>1173</v>
       </c>
-      <c r="G592" t="s">
-        <v>23</v>
-      </c>
       <c r="H592" t="s">
         <v>23</v>
       </c>
@@ -23314,9 +23272,6 @@
       <c r="I640" t="s">
         <v>48</v>
       </c>
-      <c r="J640" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="641">
       <c r="A641" t="s">
@@ -23377,9 +23332,6 @@
       <c r="I643" t="s">
         <v>48</v>
       </c>
-      <c r="J643" t="s">
-        <v>48</v>
-      </c>
       <c r="L643" t="s">
         <v>48</v>
       </c>
@@ -23926,9 +23878,6 @@
       <c r="E670" t="s">
         <v>1328</v>
       </c>
-      <c r="H670" t="s">
-        <v>23</v>
-      </c>
       <c r="I670" t="s">
         <v>23</v>
       </c>
@@ -25204,9 +25153,6 @@
       <c r="E727" t="s">
         <v>1438</v>
       </c>
-      <c r="H727" t="s">
-        <v>23</v>
-      </c>
       <c r="I727" t="s">
         <v>23</v>
       </c>
@@ -26006,9 +25952,6 @@
       <c r="J762" t="s">
         <v>23</v>
       </c>
-      <c r="K762" t="s">
-        <v>23</v>
-      </c>
       <c r="L762" t="s">
         <v>23</v>
       </c>
@@ -26198,12 +26141,6 @@
       <c r="E771" t="s">
         <v>1526</v>
       </c>
-      <c r="H771" t="s">
-        <v>48</v>
-      </c>
-      <c r="I771" t="s">
-        <v>48</v>
-      </c>
       <c r="J771" t="s">
         <v>48</v>
       </c>
@@ -27080,9 +27017,6 @@
       <c r="J810" t="s">
         <v>23</v>
       </c>
-      <c r="K810" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="811">
       <c r="A811" t="s">
@@ -27200,9 +27134,6 @@
       <c r="E816" t="s">
         <v>1615</v>
       </c>
-      <c r="I816" t="s">
-        <v>48</v>
-      </c>
       <c r="J816" t="s">
         <v>48</v>
       </c>
@@ -27427,9 +27358,6 @@
       <c r="J826" t="s">
         <v>48</v>
       </c>
-      <c r="K826" t="s">
-        <v>48</v>
-      </c>
       <c r="L826" t="s">
         <v>48</v>
       </c>
@@ -27696,9 +27624,6 @@
       <c r="E839" t="s">
         <v>1655</v>
       </c>
-      <c r="I839" t="s">
-        <v>23</v>
-      </c>
       <c r="J839" t="s">
         <v>23</v>
       </c>
@@ -28146,9 +28071,6 @@
       <c r="L860" t="s">
         <v>48</v>
       </c>
-      <c r="M860" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="861">
       <c r="A861" t="s">
@@ -29484,9 +29406,6 @@
       <c r="L917" t="s">
         <v>23</v>
       </c>
-      <c r="M917" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="918">
       <c r="A918" t="s">
@@ -29556,9 +29475,6 @@
       <c r="L920" t="s">
         <v>23</v>
       </c>
-      <c r="M920" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="921">
       <c r="A921" t="s">
@@ -31184,9 +31100,6 @@
       <c r="E993" t="s">
         <v>1634</v>
       </c>
-      <c r="J993" t="s">
-        <v>48</v>
-      </c>
       <c r="K993" t="s">
         <v>48</v>
       </c>
@@ -33743,9 +33656,6 @@
       <c r="K1107" t="s">
         <v>48</v>
       </c>
-      <c r="M1107" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="1108">
       <c r="A1108" t="s">
@@ -33788,6 +33698,9 @@
       </c>
       <c r="E1109" t="s">
         <v>2178</v>
+      </c>
+      <c r="K1109" t="s">
+        <v>48</v>
       </c>
       <c r="L1109" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Fix: Remote lineup link now has actual json; Fix: Daily notificator, for time UTC_TIME_TO_CHANGE-1 interval fires with events every few seconds; Add: Progress bar for loading operations on lineup list; Fix: Calendar view now shows week mode by default, to reduce screen usage; Fix: ThunderLineupTxtGuesser now can skip add/remove list items and continue to work(before you have a choose - apply list fully, or one by one item in whole list, now typing - the list is skips)
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10316" uniqueCount="3035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10320" uniqueCount="3035">
   <si>
     <t>Vehicles</t>
   </si>
@@ -28071,6 +28071,9 @@
       <c r="L860" t="s">
         <v>48</v>
       </c>
+      <c r="M860" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="861">
       <c r="A861" t="s">
@@ -29406,6 +29409,9 @@
       <c r="L917" t="s">
         <v>23</v>
       </c>
+      <c r="M917" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="918">
       <c r="A918" t="s">
@@ -29475,6 +29481,9 @@
       <c r="L920" t="s">
         <v>23</v>
       </c>
+      <c r="M920" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="921">
       <c r="A921" t="s">
@@ -33654,6 +33663,9 @@
         <v>48</v>
       </c>
       <c r="K1107" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1107" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: FlexibleAdapter library instead of FastAdapter, cause it can handle collapse/expand sticky headers; Add: 2 Run configurations, to read dump files, one to read local, and second to read remotely; Add: Sticky foldable headers for lineup list;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10320" uniqueCount="3035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10336" uniqueCount="3035">
   <si>
     <t>Vehicles</t>
   </si>
@@ -19488,6 +19488,9 @@
       <c r="H473" t="s">
         <v>23</v>
       </c>
+      <c r="L473" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="474">
       <c r="A474" t="s">
@@ -21106,6 +21109,9 @@
       <c r="I544" t="s">
         <v>48</v>
       </c>
+      <c r="J544" t="s">
+        <v>48</v>
+      </c>
       <c r="K544" t="s">
         <v>48</v>
       </c>
@@ -22699,6 +22705,9 @@
       <c r="I613" t="s">
         <v>48</v>
       </c>
+      <c r="J613" t="s">
+        <v>48</v>
+      </c>
       <c r="K613" t="s">
         <v>48</v>
       </c>
@@ -26755,6 +26764,9 @@
       <c r="I799" t="s">
         <v>23</v>
       </c>
+      <c r="J799" t="s">
+        <v>23</v>
+      </c>
       <c r="K799" t="s">
         <v>23</v>
       </c>
@@ -26827,6 +26839,9 @@
       <c r="I802" t="s">
         <v>23</v>
       </c>
+      <c r="J802" t="s">
+        <v>23</v>
+      </c>
       <c r="K802" t="s">
         <v>23</v>
       </c>
@@ -28065,6 +28080,9 @@
       <c r="E860" t="s">
         <v>1695</v>
       </c>
+      <c r="J860" t="s">
+        <v>23</v>
+      </c>
       <c r="K860" t="s">
         <v>23</v>
       </c>
@@ -29403,6 +29421,9 @@
       <c r="I917" t="s">
         <v>23</v>
       </c>
+      <c r="J917" t="s">
+        <v>23</v>
+      </c>
       <c r="K917" t="s">
         <v>23</v>
       </c>
@@ -29475,6 +29496,9 @@
       <c r="E920" t="s">
         <v>1811</v>
       </c>
+      <c r="J920" t="s">
+        <v>23</v>
+      </c>
       <c r="K920" t="s">
         <v>23</v>
       </c>
@@ -30802,6 +30826,9 @@
       <c r="E979" t="s">
         <v>1926</v>
       </c>
+      <c r="J979" t="s">
+        <v>23</v>
+      </c>
       <c r="K979" t="s">
         <v>23</v>
       </c>
@@ -32335,6 +32362,9 @@
       <c r="E1048" t="s">
         <v>2058</v>
       </c>
+      <c r="J1048" t="s">
+        <v>23</v>
+      </c>
       <c r="K1048" t="s">
         <v>23</v>
       </c>
@@ -32450,6 +32480,9 @@
       <c r="E1053" t="s">
         <v>2068</v>
       </c>
+      <c r="J1053" t="s">
+        <v>48</v>
+      </c>
       <c r="K1053" t="s">
         <v>48</v>
       </c>
@@ -32473,6 +32506,9 @@
       <c r="E1054" t="s">
         <v>2070</v>
       </c>
+      <c r="J1054" t="s">
+        <v>48</v>
+      </c>
       <c r="K1054" t="s">
         <v>48</v>
       </c>
@@ -32565,6 +32601,9 @@
       <c r="E1058" t="s">
         <v>2078</v>
       </c>
+      <c r="J1058" t="s">
+        <v>23</v>
+      </c>
       <c r="K1058" t="s">
         <v>23</v>
       </c>
@@ -33613,6 +33652,9 @@
       <c r="E1105" t="s">
         <v>2170</v>
       </c>
+      <c r="J1105" t="s">
+        <v>48</v>
+      </c>
       <c r="K1105" t="s">
         <v>48</v>
       </c>
@@ -33783,6 +33825,9 @@
       <c r="E1112" t="s">
         <v>2183</v>
       </c>
+      <c r="J1112" t="s">
+        <v>23</v>
+      </c>
       <c r="K1112" t="s">
         <v>23</v>
       </c>
@@ -33805,6 +33850,9 @@
       </c>
       <c r="E1113" t="s">
         <v>2185</v>
+      </c>
+      <c r="J1113" t="s">
+        <v>23</v>
       </c>
       <c r="K1113" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Add: Firebase libs, to catch crash logs, and basic statistics; Add: New ignore endings for vehicle ids - one more amx13, and yt_cup; Add: Target/Compile sdk now is 30; Add: Change log for db update feature; Fix: getFavoriteVehicles is no more crashing NotificationWorker; Add: Calendar day decorator for today, to distinct today; Add: ExpandableHeaderItem now can work with different sub items; Add: ExpandableHeaderItem now count sub items depends on a search result; Fix: Bug with vehicle filtering, when case was not ignored;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10336" uniqueCount="3035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10333" uniqueCount="3027">
   <si>
     <t>Vehicles</t>
   </si>
@@ -2705,6 +2705,12 @@
     <t>Wellington Mk Ic</t>
   </si>
   <si>
+    <t>tbf-1c</t>
+  </si>
+  <si>
+    <t>TBF-1C Avenger</t>
+  </si>
+  <si>
     <t>p-40f_10</t>
   </si>
   <si>
@@ -2717,12 +2723,6 @@
     <t>A-36 Apache</t>
   </si>
   <si>
-    <t>tbf-1c</t>
-  </si>
-  <si>
-    <t>TBF-1C Avenger</t>
-  </si>
-  <si>
     <t>p-36g</t>
   </si>
   <si>
@@ -9050,9 +9050,6 @@
     <t>B-17G-60-VE Flying Fortress</t>
   </si>
   <si>
-    <t>us_amx_13_90</t>
-  </si>
-  <si>
     <t>b-29</t>
   </si>
   <si>
@@ -9092,31 +9089,10 @@
     <t>Tank, Combat, Full-Tracked, 105-mm Gun XM-1 (Chrysler)</t>
   </si>
   <si>
-    <t>md_460_yt_cup_2019</t>
-  </si>
-  <si>
     <t>mig-15bis_nr23_german</t>
   </si>
   <si>
     <t>md_460_usa</t>
-  </si>
-  <si>
-    <t>germ_leopard_2a5_yt_cup_2019</t>
-  </si>
-  <si>
-    <t>ussr_t_80u_yt_cup_2019</t>
-  </si>
-  <si>
-    <t>uk_challenger_II_yt_cup_2019</t>
-  </si>
-  <si>
-    <t>Challenger 2</t>
-  </si>
-  <si>
-    <t>us_m1a1_abrams_yt_cup_2019</t>
-  </si>
-  <si>
-    <t>M1A1</t>
   </si>
 </sst>
 </file>
@@ -9163,7 +9139,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" ref="A2:P1546" displayName="Test_Table" name="Test">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" ref="A2:P1540" displayName="Test_Table" name="Test">
   <tableColumns count="16">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Type"/>
@@ -9188,7 +9164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1546"/>
+  <dimension ref="A1:P1540"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -12014,6 +11990,9 @@
       <c r="F138" t="s">
         <v>48</v>
       </c>
+      <c r="G138" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
@@ -14356,6 +14335,9 @@
       <c r="G247" t="s">
         <v>48</v>
       </c>
+      <c r="H247" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
@@ -15092,6 +15074,9 @@
       <c r="G279" t="s">
         <v>23</v>
       </c>
+      <c r="H279" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
@@ -16168,6 +16153,9 @@
       <c r="E328" t="s">
         <v>667</v>
       </c>
+      <c r="F328" t="s">
+        <v>48</v>
+      </c>
       <c r="G328" t="s">
         <v>48</v>
       </c>
@@ -16197,6 +16185,9 @@
       <c r="H329" t="s">
         <v>48</v>
       </c>
+      <c r="I329" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="s">
@@ -16375,6 +16366,9 @@
       <c r="E337" t="s">
         <v>667</v>
       </c>
+      <c r="F337" t="s">
+        <v>48</v>
+      </c>
       <c r="G337" t="s">
         <v>48</v>
       </c>
@@ -17249,6 +17243,9 @@
       <c r="E375" t="s">
         <v>755</v>
       </c>
+      <c r="F375" t="s">
+        <v>23</v>
+      </c>
       <c r="G375" t="s">
         <v>23</v>
       </c>
@@ -18019,6 +18016,9 @@
       <c r="H409" t="s">
         <v>48</v>
       </c>
+      <c r="I409" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="s">
@@ -18956,6 +18956,9 @@
       <c r="E450" t="s">
         <v>898</v>
       </c>
+      <c r="F450" t="s">
+        <v>23</v>
+      </c>
       <c r="G450" t="s">
         <v>23</v>
       </c>
@@ -19806,6 +19809,9 @@
       <c r="E488" t="s">
         <v>973</v>
       </c>
+      <c r="G488" t="s">
+        <v>48</v>
+      </c>
       <c r="H488" t="s">
         <v>48</v>
       </c>
@@ -19829,6 +19835,9 @@
       <c r="E489" t="s">
         <v>975</v>
       </c>
+      <c r="G489" t="s">
+        <v>48</v>
+      </c>
       <c r="H489" t="s">
         <v>48</v>
       </c>
@@ -20223,6 +20232,9 @@
       <c r="E506" t="s">
         <v>1007</v>
       </c>
+      <c r="G506" t="s">
+        <v>23</v>
+      </c>
       <c r="H506" t="s">
         <v>23</v>
       </c>
@@ -20499,6 +20511,9 @@
       <c r="E518" t="s">
         <v>1031</v>
       </c>
+      <c r="G518" t="s">
+        <v>23</v>
+      </c>
       <c r="H518" t="s">
         <v>23</v>
       </c>
@@ -22009,6 +22024,9 @@
       <c r="E583" t="s">
         <v>1156</v>
       </c>
+      <c r="G583" t="s">
+        <v>23</v>
+      </c>
       <c r="H583" t="s">
         <v>23</v>
       </c>
@@ -22219,6 +22237,9 @@
       <c r="E592" t="s">
         <v>1173</v>
       </c>
+      <c r="G592" t="s">
+        <v>23</v>
+      </c>
       <c r="H592" t="s">
         <v>23</v>
       </c>
@@ -23281,6 +23302,9 @@
       <c r="I640" t="s">
         <v>48</v>
       </c>
+      <c r="J640" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="641">
       <c r="A641" t="s">
@@ -23341,6 +23365,9 @@
       <c r="I643" t="s">
         <v>48</v>
       </c>
+      <c r="J643" t="s">
+        <v>48</v>
+      </c>
       <c r="L643" t="s">
         <v>48</v>
       </c>
@@ -23887,6 +23914,9 @@
       <c r="E670" t="s">
         <v>1328</v>
       </c>
+      <c r="H670" t="s">
+        <v>23</v>
+      </c>
       <c r="I670" t="s">
         <v>23</v>
       </c>
@@ -25162,6 +25192,9 @@
       <c r="E727" t="s">
         <v>1438</v>
       </c>
+      <c r="H727" t="s">
+        <v>23</v>
+      </c>
       <c r="I727" t="s">
         <v>23</v>
       </c>
@@ -25961,6 +25994,9 @@
       <c r="J762" t="s">
         <v>23</v>
       </c>
+      <c r="K762" t="s">
+        <v>23</v>
+      </c>
       <c r="L762" t="s">
         <v>23</v>
       </c>
@@ -26150,6 +26186,12 @@
       <c r="E771" t="s">
         <v>1526</v>
       </c>
+      <c r="H771" t="s">
+        <v>48</v>
+      </c>
+      <c r="I771" t="s">
+        <v>48</v>
+      </c>
       <c r="J771" t="s">
         <v>48</v>
       </c>
@@ -27032,6 +27074,9 @@
       <c r="J810" t="s">
         <v>23</v>
       </c>
+      <c r="K810" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="811">
       <c r="A811" t="s">
@@ -27149,6 +27194,9 @@
       <c r="E816" t="s">
         <v>1615</v>
       </c>
+      <c r="I816" t="s">
+        <v>48</v>
+      </c>
       <c r="J816" t="s">
         <v>48</v>
       </c>
@@ -27373,6 +27421,9 @@
       <c r="J826" t="s">
         <v>48</v>
       </c>
+      <c r="K826" t="s">
+        <v>48</v>
+      </c>
       <c r="L826" t="s">
         <v>48</v>
       </c>
@@ -27639,6 +27690,9 @@
       <c r="E839" t="s">
         <v>1655</v>
       </c>
+      <c r="I839" t="s">
+        <v>23</v>
+      </c>
       <c r="J839" t="s">
         <v>23</v>
       </c>
@@ -31136,6 +31190,9 @@
       <c r="E993" t="s">
         <v>1634</v>
       </c>
+      <c r="J993" t="s">
+        <v>48</v>
+      </c>
       <c r="K993" t="s">
         <v>48</v>
       </c>
@@ -43060,7 +43117,7 @@
         <v>3012</v>
       </c>
       <c r="B1532" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="C1532" t="s">
         <v>104</v>
@@ -43069,41 +43126,41 @@
         <v>2243</v>
       </c>
       <c r="E1532" t="s">
-        <v>2246</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="1533">
       <c r="A1533" t="s">
-        <v>3013</v>
+        <v>3014</v>
       </c>
       <c r="B1533" t="s">
         <v>113</v>
       </c>
       <c r="C1533" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D1533" t="s">
-        <v>2243</v>
+        <v>2331</v>
       </c>
       <c r="E1533" t="s">
-        <v>3014</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="1534">
       <c r="A1534" t="s">
-        <v>3015</v>
+        <v>3016</v>
       </c>
       <c r="B1534" t="s">
         <v>113</v>
       </c>
       <c r="C1534" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D1534" t="s">
         <v>2331</v>
       </c>
       <c r="E1534" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="1535">
@@ -43114,81 +43171,81 @@
         <v>113</v>
       </c>
       <c r="C1535" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D1535" t="s">
         <v>2331</v>
       </c>
       <c r="E1535" t="s">
-        <v>3016</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="1536">
       <c r="A1536" t="s">
-        <v>3018</v>
+        <v>3019</v>
       </c>
       <c r="B1536" t="s">
         <v>113</v>
       </c>
       <c r="C1536" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D1536" t="s">
         <v>2331</v>
       </c>
       <c r="E1536" t="s">
-        <v>3019</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="1537">
       <c r="A1537" t="s">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="B1537" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C1537" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D1537" t="s">
-        <v>2331</v>
+        <v>2528</v>
       </c>
       <c r="E1537" t="s">
-        <v>3021</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="1538">
       <c r="A1538" t="s">
-        <v>3022</v>
+        <v>3023</v>
       </c>
       <c r="B1538" t="s">
         <v>19</v>
       </c>
       <c r="C1538" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D1538" t="s">
-        <v>2528</v>
+        <v>2650</v>
       </c>
       <c r="E1538" t="s">
-        <v>3023</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="1539">
       <c r="A1539" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="B1539" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="C1539" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="D1539" t="s">
         <v>2650</v>
       </c>
       <c r="E1539" t="s">
-        <v>3025</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="1540">
@@ -43199,115 +43256,13 @@
         <v>113</v>
       </c>
       <c r="C1540" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="D1540" t="s">
         <v>2650</v>
       </c>
       <c r="E1540" t="s">
         <v>2687</v>
-      </c>
-    </row>
-    <row r="1541">
-      <c r="A1541" t="s">
-        <v>3027</v>
-      </c>
-      <c r="B1541" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1541" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1541" t="s">
-        <v>2650</v>
-      </c>
-      <c r="E1541" t="s">
-        <v>2634</v>
-      </c>
-    </row>
-    <row r="1542">
-      <c r="A1542" t="s">
-        <v>3028</v>
-      </c>
-      <c r="B1542" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1542" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1542" t="s">
-        <v>2650</v>
-      </c>
-      <c r="E1542" t="s">
-        <v>2687</v>
-      </c>
-    </row>
-    <row r="1543">
-      <c r="A1543" t="s">
-        <v>3029</v>
-      </c>
-      <c r="B1543" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1543" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1543" t="s">
-        <v>2941</v>
-      </c>
-      <c r="E1543" t="s">
-        <v>2880</v>
-      </c>
-    </row>
-    <row r="1544">
-      <c r="A1544" t="s">
-        <v>3030</v>
-      </c>
-      <c r="B1544" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1544" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1544" t="s">
-        <v>2941</v>
-      </c>
-      <c r="E1544" t="s">
-        <v>2946</v>
-      </c>
-    </row>
-    <row r="1545">
-      <c r="A1545" t="s">
-        <v>3031</v>
-      </c>
-      <c r="B1545" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1545" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1545" t="s">
-        <v>2941</v>
-      </c>
-      <c r="E1545" t="s">
-        <v>3032</v>
-      </c>
-    </row>
-    <row r="1546">
-      <c r="A1546" t="s">
-        <v>3033</v>
-      </c>
-      <c r="B1546" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1546" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1546" t="s">
-        <v>2941</v>
-      </c>
-      <c r="E1546" t="s">
-        <v>3034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: actual lineups: Infanterikanonvagn 73 is added to 2_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10445" uniqueCount="3073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10446" uniqueCount="3073">
   <si>
     <t>Vehicles</t>
   </si>
@@ -19984,6 +19984,9 @@
       <c r="E490" t="s">
         <v>979</v>
       </c>
+      <c r="G490" t="s">
+        <v>23</v>
+      </c>
       <c r="H490" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Add: actual lineups vesion==11: Semovente M42 Contraereo is added to 8_2 OTO R3 T20 FA-HS is added to 8_2
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10446" uniqueCount="3073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10448" uniqueCount="3073">
   <si>
     <t>Vehicles</t>
   </si>
@@ -21508,6 +21508,9 @@
       <c r="K556" t="s">
         <v>48</v>
       </c>
+      <c r="L556" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="557">
       <c r="A557" t="s">
@@ -22961,6 +22964,9 @@
         <v>48</v>
       </c>
       <c r="K619" t="s">
+        <v>48</v>
+      </c>
+      <c r="L619" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Found dump where lineup distance was less 413 bytes, but my limit is 500, so no one of new dumps parsed correctly, now max dist is 400; Add: Dump files are sorted by date now before showing it to a user; Add: Vehicles from starteg maraphone added to xlsx;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10461" uniqueCount="3077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10476" uniqueCount="3083">
   <si>
     <t>Vehicles</t>
   </si>
@@ -9146,6 +9146,12 @@
     <t>cn_type_95_ha_go</t>
   </si>
   <si>
+    <t>germ_sdkfz_251_10</t>
+  </si>
+  <si>
+    <t>m.Schütz.Pz.Wg. (Sd.Kfz.251/10)</t>
+  </si>
+  <si>
     <t>sw_strv_m39_td</t>
   </si>
   <si>
@@ -9194,6 +9200,12 @@
     <t>G8N1 Renzan</t>
   </si>
   <si>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
     <t>b-17g</t>
   </si>
   <si>
@@ -9243,6 +9255,12 @@
   </si>
   <si>
     <t>md_460_usa</t>
+  </si>
+  <si>
+    <t>us_merkava_mk_3d</t>
+  </si>
+  <si>
+    <t>Merkava Mk.3D</t>
   </si>
 </sst>
 </file>
@@ -9289,7 +9307,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" ref="A2:P1564" displayName="Test_Table" name="Test">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" ref="A2:P1567" displayName="Test_Table" name="Test">
   <tableColumns count="16">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Type"/>
@@ -9314,7 +9332,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1564"/>
+  <dimension ref="A1:P1567"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -43515,7 +43533,7 @@
         <v>19</v>
       </c>
       <c r="C1545" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="D1545" t="s">
         <v>21</v>
@@ -43532,10 +43550,10 @@
         <v>19</v>
       </c>
       <c r="C1546" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D1546" t="s">
-        <v>202</v>
+        <v>21</v>
       </c>
       <c r="E1546" t="s">
         <v>3047</v>
@@ -43549,10 +43567,10 @@
         <v>19</v>
       </c>
       <c r="C1547" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D1547" t="s">
-        <v>602</v>
+        <v>202</v>
       </c>
       <c r="E1547" t="s">
         <v>3049</v>
@@ -43566,18 +43584,18 @@
         <v>19</v>
       </c>
       <c r="C1548" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="D1548" t="s">
         <v>602</v>
       </c>
       <c r="E1548" t="s">
-        <v>3049</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="1549">
       <c r="A1549" t="s">
-        <v>3051</v>
+        <v>3052</v>
       </c>
       <c r="B1549" t="s">
         <v>19</v>
@@ -43589,41 +43607,41 @@
         <v>602</v>
       </c>
       <c r="E1549" t="s">
-        <v>2190</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="1550">
       <c r="A1550" t="s">
-        <v>3052</v>
+        <v>3053</v>
       </c>
       <c r="B1550" t="s">
         <v>19</v>
       </c>
       <c r="C1550" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D1550" t="s">
         <v>602</v>
       </c>
       <c r="E1550" t="s">
-        <v>3049</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="1551">
       <c r="A1551" t="s">
-        <v>3053</v>
+        <v>3054</v>
       </c>
       <c r="B1551" t="s">
         <v>19</v>
       </c>
       <c r="C1551" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D1551" t="s">
-        <v>795</v>
+        <v>602</v>
       </c>
       <c r="E1551" t="s">
-        <v>3054</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="1552">
@@ -43634,10 +43652,10 @@
         <v>19</v>
       </c>
       <c r="C1552" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="D1552" t="s">
-        <v>1208</v>
+        <v>795</v>
       </c>
       <c r="E1552" t="s">
         <v>3056</v>
@@ -43654,27 +43672,27 @@
         <v>107</v>
       </c>
       <c r="D1553" t="s">
-        <v>1701</v>
+        <v>1208</v>
       </c>
       <c r="E1553" t="s">
-        <v>1619</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="1554">
       <c r="A1554" t="s">
-        <v>3058</v>
+        <v>3059</v>
       </c>
       <c r="B1554" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="C1554" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="D1554" t="s">
-        <v>2165</v>
+        <v>1701</v>
       </c>
       <c r="E1554" t="s">
-        <v>3059</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="1555">
@@ -43685,7 +43703,7 @@
         <v>126</v>
       </c>
       <c r="C1555" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D1555" t="s">
         <v>2165</v>
@@ -43702,10 +43720,10 @@
         <v>126</v>
       </c>
       <c r="C1556" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D1556" t="s">
-        <v>2274</v>
+        <v>2165</v>
       </c>
       <c r="E1556" t="s">
         <v>3063</v>
@@ -43719,10 +43737,10 @@
         <v>126</v>
       </c>
       <c r="C1557" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="D1557" t="s">
-        <v>2364</v>
+        <v>2165</v>
       </c>
       <c r="E1557" t="s">
         <v>3065</v>
@@ -43736,47 +43754,47 @@
         <v>126</v>
       </c>
       <c r="C1558" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="D1558" t="s">
-        <v>2364</v>
+        <v>2274</v>
       </c>
       <c r="E1558" t="s">
-        <v>3065</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="1559">
       <c r="A1559" t="s">
-        <v>3067</v>
+        <v>3068</v>
       </c>
       <c r="B1559" t="s">
         <v>126</v>
       </c>
       <c r="C1559" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="D1559" t="s">
         <v>2364</v>
       </c>
       <c r="E1559" t="s">
-        <v>3068</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="1560">
       <c r="A1560" t="s">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="B1560" t="s">
         <v>126</v>
       </c>
       <c r="C1560" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D1560" t="s">
         <v>2364</v>
       </c>
       <c r="E1560" t="s">
-        <v>3070</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="1561">
@@ -43784,13 +43802,13 @@
         <v>3071</v>
       </c>
       <c r="B1561" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="C1561" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="D1561" t="s">
-        <v>2554</v>
+        <v>2364</v>
       </c>
       <c r="E1561" t="s">
         <v>3072</v>
@@ -43804,47 +43822,98 @@
         <v>126</v>
       </c>
       <c r="C1562" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D1562" t="s">
-        <v>2630</v>
+        <v>2364</v>
       </c>
       <c r="E1562" t="s">
-        <v>2677</v>
+        <v>3074</v>
       </c>
     </row>
     <row r="1563">
       <c r="A1563" t="s">
-        <v>3074</v>
+        <v>3075</v>
       </c>
       <c r="B1563" t="s">
         <v>19</v>
       </c>
       <c r="C1563" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="D1563" t="s">
-        <v>2698</v>
+        <v>2554</v>
       </c>
       <c r="E1563" t="s">
-        <v>3075</v>
+        <v>3076</v>
       </c>
     </row>
     <row r="1564">
       <c r="A1564" t="s">
-        <v>3076</v>
+        <v>3077</v>
       </c>
       <c r="B1564" t="s">
         <v>126</v>
       </c>
       <c r="C1564" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1564" t="s">
+        <v>2630</v>
+      </c>
+      <c r="E1564" t="s">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="1565">
+      <c r="A1565" t="s">
+        <v>3078</v>
+      </c>
+      <c r="B1565" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1565" t="s">
         <v>116</v>
       </c>
-      <c r="D1564" t="s">
+      <c r="D1565" t="s">
         <v>2698</v>
       </c>
-      <c r="E1564" t="s">
+      <c r="E1565" t="s">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="1566">
+      <c r="A1566" t="s">
+        <v>3080</v>
+      </c>
+      <c r="B1566" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1566" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1566" t="s">
+        <v>2698</v>
+      </c>
+      <c r="E1566" t="s">
         <v>2731</v>
+      </c>
+    </row>
+    <row r="1567">
+      <c r="A1567" t="s">
+        <v>3081</v>
+      </c>
+      <c r="B1567" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1567" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1567" t="s">
+        <v>2951</v>
+      </c>
+      <c r="E1567" t="s">
+        <v>3082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: actual lineup 8_2 has lost JsonVehicle(name=us_t26e4_superpershing, type=TANK, nation=US, br=6.3, locale=JsonLocaleItem(id=us_t26e4_superpershing, title=Heavy Tank T26E1-1 "Super Pershing", nation=US));
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10476" uniqueCount="3083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10475" uniqueCount="3083">
   <si>
     <t>Vehicles</t>
   </si>
@@ -33409,9 +33409,6 @@
       <c r="K1087" t="s">
         <v>23</v>
       </c>
-      <c r="L1087" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="1088">
       <c r="A1088" t="s">

</xml_diff>

<commit_message>
Add: Actual lineups: OTO R3 T20 FA-HS(IT) is deleted from 3_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10875" uniqueCount="3204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10874" uniqueCount="3204">
   <si>
     <t>Vehicles</t>
   </si>
@@ -4244,16 +4244,16 @@
     <t>Pz.Kpfw. IV Ausf. H</t>
   </si>
   <si>
+    <t>it_semovente_breda_501</t>
+  </si>
+  <si>
+    <t>Semovente Ruotato da 90/52 Breda 501</t>
+  </si>
+  <si>
     <t>it_oto_r3_t20_fa</t>
   </si>
   <si>
     <t>OTO R3 T20 FA-HS</t>
-  </si>
-  <si>
-    <t>it_semovente_breda_501</t>
-  </si>
-  <si>
-    <t>Semovente Ruotato da 90/52 Breda 501</t>
   </si>
   <si>
     <t>jp_type_3_chi_nu_75cm_type_5</t>
@@ -25302,13 +25302,10 @@
       <c r="H713" t="s">
         <v>48</v>
       </c>
+      <c r="I713" t="s">
+        <v>48</v>
+      </c>
       <c r="J713" t="s">
-        <v>48</v>
-      </c>
-      <c r="K713" t="s">
-        <v>48</v>
-      </c>
-      <c r="L713" t="s">
         <v>48</v>
       </c>
     </row>
@@ -25328,13 +25325,13 @@
       <c r="E714" t="s">
         <v>1413</v>
       </c>
-      <c r="H714" t="s">
-        <v>48</v>
-      </c>
-      <c r="I714" t="s">
-        <v>48</v>
-      </c>
       <c r="J714" t="s">
+        <v>48</v>
+      </c>
+      <c r="K714" t="s">
+        <v>48</v>
+      </c>
+      <c r="L714" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: Actual lineup changes 3 inch Gun Motor Carriage T55E1(US) is added to 4_1     ChangeAdapter: StuG III G(IT) is added to 4_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11248" uniqueCount="3311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11250" uniqueCount="3311">
   <si>
     <t>Vehicles</t>
   </si>
@@ -25861,6 +25861,9 @@
       <c r="H724" t="s">
         <v>48</v>
       </c>
+      <c r="I724" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="725">
       <c r="A725" t="s">
@@ -27765,6 +27768,9 @@
         <v>1597</v>
       </c>
       <c r="H807" t="s">
+        <v>23</v>
+      </c>
+      <c r="I807" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: actual lineup changes: Type 97 Chi-Ha Kai TD(JP) добавлен в 1_1 s.Pz.Sp.Wg. (5 cm 39/1 L60)(GR) добавлен в 1_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11351" uniqueCount="3348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11353" uniqueCount="3348">
   <si>
     <t>Vehicles</t>
   </si>
@@ -1523,6 +1523,12 @@
     <t>jp_type_97_kai</t>
   </si>
   <si>
+    <t>jp_type_97_kai_td</t>
+  </si>
+  <si>
+    <t>Type 97 Chi-Ha Kai TD</t>
+  </si>
+  <si>
     <t>jp_type_2_ho_i</t>
   </si>
   <si>
@@ -1535,12 +1541,6 @@
     <t>Type 1 Ho-Ni I</t>
   </si>
   <si>
-    <t>jp_type_97_kai_td</t>
-  </si>
-  <si>
-    <t>Type 97 Chi-Ha Kai TD</t>
-  </si>
-  <si>
     <t>ussr_t_28</t>
   </si>
   <si>
@@ -2570,6 +2570,9 @@
     <t>s.Pz.Sp.Wg. (5 cm 39/1 L60)</t>
   </si>
   <si>
+    <t>germ_sdkfz_234_2_td</t>
+  </si>
+  <si>
     <t>germ_pzkpfw_III_ausf_J</t>
   </si>
   <si>
@@ -2580,9 +2583,6 @@
   </si>
   <si>
     <t>Pz.III J1 TD</t>
-  </si>
-  <si>
-    <t>germ_sdkfz_234_2_td</t>
   </si>
   <si>
     <t>jp_navy_120mm_spg</t>
@@ -15206,6 +15206,9 @@
       <c r="E243" t="s">
         <v>504</v>
       </c>
+      <c r="F243" t="s">
+        <v>48</v>
+      </c>
       <c r="G243" t="s">
         <v>48</v>
       </c>
@@ -19300,7 +19303,10 @@
         <v>848</v>
       </c>
       <c r="E425" t="s">
-        <v>853</v>
+        <v>851</v>
+      </c>
+      <c r="F425" t="s">
+        <v>48</v>
       </c>
       <c r="G425" t="s">
         <v>48</v>
@@ -19308,7 +19314,7 @@
     </row>
     <row r="426">
       <c r="A426" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B426" t="s">
         <v>19</v>
@@ -19320,7 +19326,7 @@
         <v>848</v>
       </c>
       <c r="E426" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G426" t="s">
         <v>48</v>
@@ -19328,7 +19334,7 @@
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B427" t="s">
         <v>19</v>
@@ -19340,7 +19346,7 @@
         <v>848</v>
       </c>
       <c r="E427" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="G427" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add: Actual lineup: SU-76D(RU) is added to 3_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11353" uniqueCount="3348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11354" uniqueCount="3348">
   <si>
     <t>Vehicles</t>
   </si>
@@ -17304,6 +17304,9 @@
       <c r="G338" t="s">
         <v>23</v>
       </c>
+      <c r="H338" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="s">

</xml_diff>

<commit_message>
Add: Ystervark(UK) is added to 5_1          Assault tank T26E5(US) is added to 5_1          PT-76-57(RU) is added to 5_1          So-Ki(JP) is deleted from 5_1          STB-1(JP) is deleted from 9_2;
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11883" uniqueCount="3510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11884" uniqueCount="3510">
   <si>
     <t>Vehicles</t>
   </si>
@@ -6782,18 +6782,18 @@
     <t>Medium Tank M26E1</t>
   </si>
   <si>
+    <t>us_t26e5</t>
+  </si>
+  <si>
+    <t>Assault tank T26E5</t>
+  </si>
+  <si>
     <t>us_m26_t99</t>
   </si>
   <si>
     <t>Medium Tank M26 T99</t>
   </si>
   <si>
-    <t>us_t26e5</t>
-  </si>
-  <si>
-    <t>Assault tank T26E5</t>
-  </si>
-  <si>
     <t>la-9_china</t>
   </si>
   <si>
@@ -7226,16 +7226,16 @@
     <t>Type 60 ATM</t>
   </si>
   <si>
+    <t>ussr_pt_76_57</t>
+  </si>
+  <si>
+    <t>PT-76-57</t>
+  </si>
+  <si>
     <t>ussr_t_44_100</t>
   </si>
   <si>
     <t>T-44-100</t>
-  </si>
-  <si>
-    <t>ussr_pt_76_57</t>
-  </si>
-  <si>
-    <t>PT-76-57</t>
   </si>
   <si>
     <t>ussr_is_3</t>
@@ -22121,9 +22121,6 @@
       <c r="I528" t="s">
         <v>48</v>
       </c>
-      <c r="J528" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="529">
       <c r="A529" t="s">
@@ -28901,6 +28898,9 @@
       <c r="I831" t="s">
         <v>23</v>
       </c>
+      <c r="J831" t="s">
+        <v>23</v>
+      </c>
       <c r="K831" t="s">
         <v>23</v>
       </c>
@@ -36078,6 +36078,9 @@
       <c r="E1151" t="s">
         <v>2257</v>
       </c>
+      <c r="J1151" t="s">
+        <v>23</v>
+      </c>
       <c r="K1151" t="s">
         <v>23</v>
       </c>
@@ -37743,6 +37746,9 @@
       <c r="E1226" t="s">
         <v>2405</v>
       </c>
+      <c r="J1226" t="s">
+        <v>23</v>
+      </c>
       <c r="K1226" t="s">
         <v>23</v>
       </c>
@@ -40466,9 +40472,6 @@
         <v>2648</v>
       </c>
       <c r="M1348" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1348" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: PT-76-57(RU) удален из 5_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12245" uniqueCount="3625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12244" uniqueCount="3625">
   <si>
     <t>Vehicles</t>
   </si>
@@ -39368,9 +39368,6 @@
       <c r="E1284" t="s">
         <v>2520</v>
       </c>
-      <c r="J1284" t="s">
-        <v>23</v>
-      </c>
       <c r="K1284" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Add: Alecto I(UK) добавлен в 1_1      M64(CH) добавлен в 3_1      Su-8(RU) добавлен в 8_2      T-55AMD-1(RU) добавлен в 9_2      ZTZ88A(CH) добавлен в 9_2      T-72M2(RU) добавлен в 10_2      Kfir C.2(IL) добавлен в 10_2      S-199(IL) удален из 4_1      M-51 (W)(IL) удален из 4_1
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12626" uniqueCount="3744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12627" uniqueCount="3744">
   <si>
     <t>Vehicles</t>
   </si>
@@ -30444,6 +30444,9 @@
       <c r="H872" t="s">
         <v>23</v>
       </c>
+      <c r="J872" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="873">
       <c r="A873" t="s">

</xml_diff>